<commit_message>
Added functions to check answers in question lookup
</commit_message>
<xml_diff>
--- a/data/fff-question-lookup.xlsx
+++ b/data/fff-question-lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/FFF-RedCap/FFF-RedCap-data-processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1154" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D24017C7-F90E-402D-9124-9ABFD093165F}"/>
+  <xr:revisionPtr revIDLastSave="1157" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58032DFA-C0C7-4CBF-BF57-D8E6476E65A6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-5520" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2340,9 +2340,6 @@
     <t>Yes; No</t>
   </si>
   <si>
-    <t>FFF_option_code</t>
-  </si>
-  <si>
     <t>1; 0</t>
   </si>
   <si>
@@ -2626,6 +2623,9 @@
   </si>
   <si>
     <t>Hardly ever or never; Some of the time; Often</t>
+  </si>
+  <si>
+    <t>RC_option_code</t>
   </si>
 </sst>
 </file>
@@ -2979,7 +2979,7 @@
   <dimension ref="A1:F367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3009,7 +3009,7 @@
         <v>753</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>756</v>
+        <v>851</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3164,7 +3164,7 @@
         <v>755</v>
       </c>
       <c r="F11" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3223,7 +3223,7 @@
         <v>431</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F15" s="6">
         <v>2</v>
@@ -3257,10 +3257,10 @@
         <v>433</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F17" t="s">
         <v>759</v>
-      </c>
-      <c r="F17" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -3280,7 +3280,7 @@
         <v>755</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3297,10 +3297,10 @@
         <v>433</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F19" t="s">
         <v>759</v>
-      </c>
-      <c r="F19" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -3418,7 +3418,7 @@
         <v>755</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3463,10 +3463,10 @@
         <v>433</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F30" t="s">
         <v>759</v>
-      </c>
-      <c r="F30" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3483,10 +3483,10 @@
         <v>444</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>761</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
@@ -3503,10 +3503,10 @@
         <v>445</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>763</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3537,10 +3537,10 @@
         <v>447</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>766</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3554,13 +3554,13 @@
         <v>399</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -3591,10 +3591,10 @@
         <v>449</v>
       </c>
       <c r="E37" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>769</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3625,10 +3625,10 @@
         <v>451</v>
       </c>
       <c r="E39" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>766</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3645,7 +3645,7 @@
         <v>453</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F40" s="4">
         <v>1</v>
@@ -3665,7 +3665,7 @@
         <v>454</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F41" s="4">
         <v>1</v>
@@ -3685,7 +3685,7 @@
         <v>455</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F42" s="4">
         <v>1</v>
@@ -3705,7 +3705,7 @@
         <v>456</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F43" s="4">
         <v>1</v>
@@ -3725,7 +3725,7 @@
         <v>457</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
@@ -3745,7 +3745,7 @@
         <v>458</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F45" s="4">
         <v>1</v>
@@ -3765,7 +3765,7 @@
         <v>459</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F46" s="4">
         <v>1</v>
@@ -3785,10 +3785,10 @@
         <v>460</v>
       </c>
       <c r="E47" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>771</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3805,10 +3805,10 @@
         <v>461</v>
       </c>
       <c r="E48" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>773</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3825,10 +3825,10 @@
         <v>463</v>
       </c>
       <c r="E49" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>766</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3845,7 +3845,7 @@
         <v>465</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F50" s="4">
         <v>1</v>
@@ -3865,7 +3865,7 @@
         <v>466</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F51" s="4">
         <v>1</v>
@@ -3885,7 +3885,7 @@
         <v>467</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F52" s="4">
         <v>1</v>
@@ -3905,7 +3905,7 @@
         <v>468</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F53" s="4">
         <v>1</v>
@@ -3925,7 +3925,7 @@
         <v>469</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F54" s="4">
         <v>1</v>
@@ -3945,7 +3945,7 @@
         <v>470</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F55" s="4">
         <v>1</v>
@@ -3965,7 +3965,7 @@
         <v>471</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F56" s="4">
         <v>1</v>
@@ -3985,10 +3985,10 @@
         <v>460</v>
       </c>
       <c r="E57" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>771</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4008,7 +4008,7 @@
         <v>755</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4028,7 +4028,7 @@
         <v>755</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4048,7 +4048,7 @@
         <v>755</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4068,7 +4068,7 @@
         <v>755</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4088,7 +4088,7 @@
         <v>755</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4108,7 +4108,7 @@
         <v>755</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4128,7 +4128,7 @@
         <v>755</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4148,7 +4148,7 @@
         <v>755</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4168,7 +4168,7 @@
         <v>755</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4188,7 +4188,7 @@
         <v>755</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4208,7 +4208,7 @@
         <v>755</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4228,7 +4228,7 @@
         <v>755</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4248,7 +4248,7 @@
         <v>755</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4268,7 +4268,7 @@
         <v>755</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4288,7 +4288,7 @@
         <v>755</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4308,7 +4308,7 @@
         <v>755</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4328,7 +4328,7 @@
         <v>755</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4348,7 +4348,7 @@
         <v>755</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4368,7 +4368,7 @@
         <v>755</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4388,7 +4388,7 @@
         <v>755</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -4408,7 +4408,7 @@
         <v>755</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
@@ -4425,10 +4425,10 @@
         <v>495</v>
       </c>
       <c r="E79" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="F79" s="3" t="s">
         <v>775</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4448,7 +4448,7 @@
         <v>755</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
@@ -4465,10 +4465,10 @@
         <v>495</v>
       </c>
       <c r="E81" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>775</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4488,7 +4488,7 @@
         <v>755</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
@@ -4505,10 +4505,10 @@
         <v>495</v>
       </c>
       <c r="E83" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>775</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -4525,10 +4525,10 @@
         <v>497</v>
       </c>
       <c r="E84" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>777</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
@@ -4545,10 +4545,10 @@
         <v>498</v>
       </c>
       <c r="E85" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>779</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4565,10 +4565,10 @@
         <v>499</v>
       </c>
       <c r="E86" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="F86" s="3" t="s">
         <v>781</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -4599,10 +4599,10 @@
         <v>502</v>
       </c>
       <c r="E88" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="F88" s="3" t="s">
         <v>783</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -4636,7 +4636,7 @@
         <v>755</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -4650,13 +4650,13 @@
         <v>500</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -4717,10 +4717,10 @@
         <v>433</v>
       </c>
       <c r="E96" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F96" t="s">
         <v>759</v>
-      </c>
-      <c r="F96" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4737,10 +4737,10 @@
         <v>505</v>
       </c>
       <c r="E97" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4757,10 +4757,10 @@
         <v>506</v>
       </c>
       <c r="E98" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4777,10 +4777,10 @@
         <v>507</v>
       </c>
       <c r="E99" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4797,10 +4797,10 @@
         <v>508</v>
       </c>
       <c r="E100" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4817,10 +4817,10 @@
         <v>509</v>
       </c>
       <c r="E101" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4837,10 +4837,10 @@
         <v>510</v>
       </c>
       <c r="E102" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4857,10 +4857,10 @@
         <v>511</v>
       </c>
       <c r="E103" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F103" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4877,10 +4877,10 @@
         <v>512</v>
       </c>
       <c r="E104" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4897,10 +4897,10 @@
         <v>513</v>
       </c>
       <c r="E105" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F105" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4917,10 +4917,10 @@
         <v>514</v>
       </c>
       <c r="E106" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F106" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4937,10 +4937,10 @@
         <v>515</v>
       </c>
       <c r="E107" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F107" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F107" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4957,10 +4957,10 @@
         <v>516</v>
       </c>
       <c r="E108" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F108" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4977,10 +4977,10 @@
         <v>517</v>
       </c>
       <c r="E109" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F109" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4997,10 +4997,10 @@
         <v>518</v>
       </c>
       <c r="E110" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F110" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F110" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -5017,10 +5017,10 @@
         <v>433</v>
       </c>
       <c r="E111" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F111" t="s">
         <v>759</v>
-      </c>
-      <c r="F111" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5037,10 +5037,10 @@
         <v>519</v>
       </c>
       <c r="E112" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="F112" s="3" t="s">
         <v>789</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5057,10 +5057,10 @@
         <v>520</v>
       </c>
       <c r="E113" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="F113" s="3" t="s">
         <v>789</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5077,10 +5077,10 @@
         <v>521</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5100,7 +5100,7 @@
         <v>755</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5117,10 +5117,10 @@
         <v>523</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -5137,10 +5137,10 @@
         <v>524</v>
       </c>
       <c r="E117" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="F117" s="3" t="s">
         <v>793</v>
-      </c>
-      <c r="F117" s="3" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5157,10 +5157,10 @@
         <v>525</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5177,10 +5177,10 @@
         <v>526</v>
       </c>
       <c r="E119" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="F119" s="3" t="s">
         <v>795</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5197,10 +5197,10 @@
         <v>527</v>
       </c>
       <c r="E120" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="F120" s="3" t="s">
         <v>795</v>
-      </c>
-      <c r="F120" s="3" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5217,10 +5217,10 @@
         <v>528</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5237,10 +5237,10 @@
         <v>529</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5257,10 +5257,10 @@
         <v>530</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -5277,10 +5277,10 @@
         <v>433</v>
       </c>
       <c r="E124" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F124" t="s">
         <v>759</v>
-      </c>
-      <c r="F124" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5297,7 +5297,7 @@
         <v>532</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F125">
         <v>1</v>
@@ -5317,7 +5317,7 @@
         <v>533</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F126">
         <v>1</v>
@@ -5337,7 +5337,7 @@
         <v>534</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F127">
         <v>1</v>
@@ -5357,7 +5357,7 @@
         <v>535</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F128">
         <v>1</v>
@@ -5377,7 +5377,7 @@
         <v>536</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F129">
         <v>1</v>
@@ -5397,7 +5397,7 @@
         <v>537</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F130">
         <v>1</v>
@@ -5417,7 +5417,7 @@
         <v>538</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F131">
         <v>1</v>
@@ -5437,7 +5437,7 @@
         <v>541</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -5457,7 +5457,7 @@
         <v>540</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F133">
         <v>1</v>
@@ -5477,7 +5477,7 @@
         <v>539</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F134">
         <v>1</v>
@@ -5497,7 +5497,7 @@
         <v>543</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F135">
         <v>1</v>
@@ -5517,7 +5517,7 @@
         <v>542</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -5537,7 +5537,7 @@
         <v>544</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F137">
         <v>1</v>
@@ -5557,7 +5557,7 @@
         <v>545</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F138">
         <v>1</v>
@@ -5577,7 +5577,7 @@
         <v>546</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F139">
         <v>1</v>
@@ -5597,7 +5597,7 @@
         <v>547</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F140">
         <v>1</v>
@@ -5617,7 +5617,7 @@
         <v>548</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F141">
         <v>1</v>
@@ -5637,7 +5637,7 @@
         <v>549</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F142">
         <v>1</v>
@@ -5657,7 +5657,7 @@
         <v>550</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F143">
         <v>1</v>
@@ -5677,7 +5677,7 @@
         <v>551</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F144">
         <v>1</v>
@@ -5697,7 +5697,7 @@
         <v>552</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F145">
         <v>1</v>
@@ -5717,7 +5717,7 @@
         <v>553</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F146">
         <v>1</v>
@@ -5737,7 +5737,7 @@
         <v>471</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F147">
         <v>1</v>
@@ -5771,10 +5771,10 @@
         <v>556</v>
       </c>
       <c r="E149" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="F149" s="3" t="s">
         <v>799</v>
-      </c>
-      <c r="F149" s="3" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5805,10 +5805,10 @@
         <v>556</v>
       </c>
       <c r="E151" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="F151" s="3" t="s">
         <v>801</v>
-      </c>
-      <c r="F151" s="3" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5825,10 +5825,10 @@
         <v>560</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5845,10 +5845,10 @@
         <v>561</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="154" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5865,10 +5865,10 @@
         <v>562</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5885,10 +5885,10 @@
         <v>563</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5905,10 +5905,10 @@
         <v>564</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5925,10 +5925,10 @@
         <v>565</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5945,10 +5945,10 @@
         <v>566</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5965,10 +5965,10 @@
         <v>567</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5985,10 +5985,10 @@
         <v>568</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6005,10 +6005,10 @@
         <v>569</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -6025,10 +6025,10 @@
         <v>556</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -6045,10 +6045,10 @@
         <v>433</v>
       </c>
       <c r="E163" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F163" t="s">
         <v>759</v>
-      </c>
-      <c r="F163" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6065,10 +6065,10 @@
         <v>556</v>
       </c>
       <c r="E164" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="F164" s="3" t="s">
         <v>804</v>
-      </c>
-      <c r="F164" s="3" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6085,10 +6085,10 @@
         <v>556</v>
       </c>
       <c r="E165" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="F165" s="3" t="s">
         <v>806</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6105,7 +6105,7 @@
         <v>576</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F166">
         <v>1</v>
@@ -6125,7 +6125,7 @@
         <v>532</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F167">
         <v>1</v>
@@ -6145,7 +6145,7 @@
         <v>577</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F168">
         <v>1</v>
@@ -6165,7 +6165,7 @@
         <v>578</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F169">
         <v>1</v>
@@ -6185,7 +6185,7 @@
         <v>579</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F170">
         <v>1</v>
@@ -6205,7 +6205,7 @@
         <v>580</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F171">
         <v>1</v>
@@ -6225,7 +6225,7 @@
         <v>581</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F172">
         <v>1</v>
@@ -6245,10 +6245,10 @@
         <v>556</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6265,7 +6265,7 @@
         <v>582</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F174">
         <v>1</v>
@@ -6285,7 +6285,7 @@
         <v>583</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F175">
         <v>1</v>
@@ -6305,7 +6305,7 @@
         <v>584</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F176">
         <v>1</v>
@@ -6325,7 +6325,7 @@
         <v>585</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F177">
         <v>1</v>
@@ -6345,7 +6345,7 @@
         <v>538</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F178">
         <v>1</v>
@@ -6365,7 +6365,7 @@
         <v>586</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F179">
         <v>1</v>
@@ -6385,7 +6385,7 @@
         <v>587</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F180">
         <v>1</v>
@@ -6405,10 +6405,10 @@
         <v>433</v>
       </c>
       <c r="E181" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F181" t="s">
         <v>759</v>
-      </c>
-      <c r="F181" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6425,10 +6425,10 @@
         <v>588</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6445,10 +6445,10 @@
         <v>589</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6465,10 +6465,10 @@
         <v>590</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6485,10 +6485,10 @@
         <v>591</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6505,10 +6505,10 @@
         <v>592</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6525,10 +6525,10 @@
         <v>593</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6545,10 +6545,10 @@
         <v>594</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6565,10 +6565,10 @@
         <v>595</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6585,10 +6585,10 @@
         <v>596</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6605,10 +6605,10 @@
         <v>597</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6625,10 +6625,10 @@
         <v>598</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6648,7 +6648,7 @@
         <v>755</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -6665,10 +6665,10 @@
         <v>600</v>
       </c>
       <c r="E194" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="F194" s="3" t="s">
         <v>810</v>
-      </c>
-      <c r="F194" s="3" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
@@ -6685,10 +6685,10 @@
         <v>433</v>
       </c>
       <c r="E195" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F195" t="s">
         <v>759</v>
-      </c>
-      <c r="F195" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -6705,10 +6705,10 @@
         <v>602</v>
       </c>
       <c r="E196" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="F196" s="3" t="s">
         <v>812</v>
-      </c>
-      <c r="F196" s="3" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -6725,10 +6725,10 @@
         <v>603</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -6745,10 +6745,10 @@
         <v>604</v>
       </c>
       <c r="E198" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F198" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -6779,10 +6779,10 @@
         <v>433</v>
       </c>
       <c r="E200" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F200" t="s">
         <v>759</v>
-      </c>
-      <c r="F200" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6799,10 +6799,10 @@
         <v>606</v>
       </c>
       <c r="E201" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="F201" s="3" t="s">
         <v>815</v>
-      </c>
-      <c r="F201" s="3" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6819,10 +6819,10 @@
         <v>607</v>
       </c>
       <c r="E202" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="F202" s="3" t="s">
         <v>815</v>
-      </c>
-      <c r="F202" s="3" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="203" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6839,10 +6839,10 @@
         <v>608</v>
       </c>
       <c r="E203" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="F203" s="3" t="s">
         <v>815</v>
-      </c>
-      <c r="F203" s="3" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6859,10 +6859,10 @@
         <v>609</v>
       </c>
       <c r="E204" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="F204" s="3" t="s">
         <v>815</v>
-      </c>
-      <c r="F204" s="3" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6879,10 +6879,10 @@
         <v>610</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F205" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6899,10 +6899,10 @@
         <v>611</v>
       </c>
       <c r="E206" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F206" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6919,10 +6919,10 @@
         <v>612</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F207" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6939,10 +6939,10 @@
         <v>613</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F208" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6959,10 +6959,10 @@
         <v>617</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F209" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6979,10 +6979,10 @@
         <v>618</v>
       </c>
       <c r="E210" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -6999,10 +6999,10 @@
         <v>619</v>
       </c>
       <c r="E211" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7019,10 +7019,10 @@
         <v>621</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F212" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7039,10 +7039,10 @@
         <v>614</v>
       </c>
       <c r="E213" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="F213" s="3" t="s">
         <v>819</v>
-      </c>
-      <c r="F213" s="3" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7059,10 +7059,10 @@
         <v>615</v>
       </c>
       <c r="E214" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="F214" s="3" t="s">
         <v>819</v>
-      </c>
-      <c r="F214" s="3" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7079,10 +7079,10 @@
         <v>616</v>
       </c>
       <c r="E215" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="F215" s="3" t="s">
         <v>819</v>
-      </c>
-      <c r="F215" s="3" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7099,10 +7099,10 @@
         <v>622</v>
       </c>
       <c r="E216" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="F216" s="3" t="s">
         <v>819</v>
-      </c>
-      <c r="F216" s="3" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
@@ -7119,10 +7119,10 @@
         <v>433</v>
       </c>
       <c r="E217" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F217" t="s">
         <v>759</v>
-      </c>
-      <c r="F217" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="218" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7139,10 +7139,10 @@
         <v>623</v>
       </c>
       <c r="E218" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="F218" s="3" t="s">
         <v>821</v>
-      </c>
-      <c r="F218" s="3" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="219" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7159,10 +7159,10 @@
         <v>624</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F219" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="220" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7179,10 +7179,10 @@
         <v>625</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F220" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7199,10 +7199,10 @@
         <v>626</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F221" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="222" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7219,10 +7219,10 @@
         <v>627</v>
       </c>
       <c r="E222" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="F222" s="3" t="s">
         <v>821</v>
-      </c>
-      <c r="F222" s="3" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="223" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7239,10 +7239,10 @@
         <v>628</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F223" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7259,10 +7259,10 @@
         <v>629</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -7279,10 +7279,10 @@
         <v>630</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F225" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7299,10 +7299,10 @@
         <v>631</v>
       </c>
       <c r="E226" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F226" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F226" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7319,10 +7319,10 @@
         <v>632</v>
       </c>
       <c r="E227" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F227" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F227" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7339,10 +7339,10 @@
         <v>636</v>
       </c>
       <c r="E228" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F228" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F228" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7359,10 +7359,10 @@
         <v>635</v>
       </c>
       <c r="E229" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F229" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F229" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="230" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7379,10 +7379,10 @@
         <v>633</v>
       </c>
       <c r="E230" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F230" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F230" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7399,10 +7399,10 @@
         <v>634</v>
       </c>
       <c r="E231" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F231" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F231" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7419,10 +7419,10 @@
         <v>637</v>
       </c>
       <c r="E232" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F232" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F232" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7439,10 +7439,10 @@
         <v>638</v>
       </c>
       <c r="E233" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F233" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F233" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7459,10 +7459,10 @@
         <v>639</v>
       </c>
       <c r="E234" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F234" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F234" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="235" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7479,10 +7479,10 @@
         <v>640</v>
       </c>
       <c r="E235" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F235" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F235" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="236" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7499,10 +7499,10 @@
         <v>641</v>
       </c>
       <c r="E236" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F236" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
@@ -7519,10 +7519,10 @@
         <v>433</v>
       </c>
       <c r="E237" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F237" t="s">
         <v>759</v>
-      </c>
-      <c r="F237" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="238" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7536,13 +7536,13 @@
         <v>410</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E238" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="F238" s="3" t="s">
         <v>821</v>
-      </c>
-      <c r="F238" s="3" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7556,13 +7556,13 @@
         <v>410</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F239" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7579,10 +7579,10 @@
         <v>642</v>
       </c>
       <c r="E240" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="F240" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="241" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7599,10 +7599,10 @@
         <v>643</v>
       </c>
       <c r="E241" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F241" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="242" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7619,10 +7619,10 @@
         <v>644</v>
       </c>
       <c r="E242" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F242" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F242" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="243" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7639,10 +7639,10 @@
         <v>645</v>
       </c>
       <c r="E243" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F243" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F243" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="244" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7659,10 +7659,10 @@
         <v>646</v>
       </c>
       <c r="E244" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F244" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F244" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="245" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7679,10 +7679,10 @@
         <v>647</v>
       </c>
       <c r="E245" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F245" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F245" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="246" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7699,10 +7699,10 @@
         <v>648</v>
       </c>
       <c r="E246" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F246" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F246" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="247" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7719,10 +7719,10 @@
         <v>649</v>
       </c>
       <c r="E247" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F247" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F247" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="248" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7739,10 +7739,10 @@
         <v>650</v>
       </c>
       <c r="E248" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F248" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F248" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="249" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7759,10 +7759,10 @@
         <v>651</v>
       </c>
       <c r="E249" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F249" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F249" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="250" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7779,10 +7779,10 @@
         <v>639</v>
       </c>
       <c r="E250" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F250" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F250" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -7799,10 +7799,10 @@
         <v>652</v>
       </c>
       <c r="E251" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F251" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="F251" s="3" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="252" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7819,10 +7819,10 @@
         <v>653</v>
       </c>
       <c r="E252" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F252" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
@@ -7839,10 +7839,10 @@
         <v>433</v>
       </c>
       <c r="E253" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F253" t="s">
         <v>759</v>
-      </c>
-      <c r="F253" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="254" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7859,10 +7859,10 @@
         <v>556</v>
       </c>
       <c r="E254" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F254" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
@@ -7879,10 +7879,10 @@
         <v>556</v>
       </c>
       <c r="E255" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="F255" s="3" t="s">
         <v>832</v>
-      </c>
-      <c r="F255" s="3" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -7899,7 +7899,7 @@
         <v>658</v>
       </c>
       <c r="E256" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F256">
         <v>1</v>
@@ -7919,7 +7919,7 @@
         <v>659</v>
       </c>
       <c r="E257" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F257">
         <v>1</v>
@@ -7939,7 +7939,7 @@
         <v>660</v>
       </c>
       <c r="E258" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F258">
         <v>1</v>
@@ -7959,7 +7959,7 @@
         <v>661</v>
       </c>
       <c r="E259" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F259">
         <v>2</v>
@@ -7979,7 +7979,7 @@
         <v>664</v>
       </c>
       <c r="E260" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F260">
         <v>3</v>
@@ -7999,7 +7999,7 @@
         <v>662</v>
       </c>
       <c r="E261" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F261">
         <v>4</v>
@@ -8019,7 +8019,7 @@
         <v>663</v>
       </c>
       <c r="E262" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F262">
         <v>5</v>
@@ -8039,7 +8039,7 @@
         <v>665</v>
       </c>
       <c r="E263" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F263">
         <v>6</v>
@@ -8073,10 +8073,10 @@
         <v>556</v>
       </c>
       <c r="E265" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F265" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.3">
@@ -8093,10 +8093,10 @@
         <v>433</v>
       </c>
       <c r="E266" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F266" t="s">
         <v>759</v>
-      </c>
-      <c r="F266" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="267" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8113,10 +8113,10 @@
         <v>667</v>
       </c>
       <c r="E267" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="F267" s="3" t="s">
         <v>812</v>
-      </c>
-      <c r="F267" s="3" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="268" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -8133,10 +8133,10 @@
         <v>668</v>
       </c>
       <c r="E268" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="F268" s="3" t="s">
         <v>834</v>
-      </c>
-      <c r="F268" s="3" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="269" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8153,10 +8153,10 @@
         <v>669</v>
       </c>
       <c r="E269" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F269" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="270" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8173,10 +8173,10 @@
         <v>670</v>
       </c>
       <c r="E270" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F270" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="271" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8207,10 +8207,10 @@
         <v>433</v>
       </c>
       <c r="E272" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F272" t="s">
         <v>759</v>
-      </c>
-      <c r="F272" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="273" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8227,10 +8227,10 @@
         <v>672</v>
       </c>
       <c r="E273" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F273" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F273" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="274" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8247,10 +8247,10 @@
         <v>673</v>
       </c>
       <c r="E274" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F274" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F274" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="275" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8267,10 +8267,10 @@
         <v>674</v>
       </c>
       <c r="E275" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F275" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F275" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="276" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8287,10 +8287,10 @@
         <v>675</v>
       </c>
       <c r="E276" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F276" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F276" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="277" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8307,10 +8307,10 @@
         <v>676</v>
       </c>
       <c r="E277" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F277" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F277" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="278" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8327,10 +8327,10 @@
         <v>677</v>
       </c>
       <c r="E278" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F278" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F278" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="279" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8347,10 +8347,10 @@
         <v>678</v>
       </c>
       <c r="E279" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F279" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F279" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="280" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8367,10 +8367,10 @@
         <v>679</v>
       </c>
       <c r="E280" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F280" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F280" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="281" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8387,10 +8387,10 @@
         <v>680</v>
       </c>
       <c r="E281" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F281" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F281" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="282" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8407,10 +8407,10 @@
         <v>681</v>
       </c>
       <c r="E282" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F282" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F282" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="283" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8427,10 +8427,10 @@
         <v>682</v>
       </c>
       <c r="E283" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F283" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F283" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="284" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8447,10 +8447,10 @@
         <v>683</v>
       </c>
       <c r="E284" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F284" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F284" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="285" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8467,10 +8467,10 @@
         <v>684</v>
       </c>
       <c r="E285" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F285" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F285" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="286" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8487,10 +8487,10 @@
         <v>685</v>
       </c>
       <c r="E286" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F286" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="F286" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.3">
@@ -8507,10 +8507,10 @@
         <v>433</v>
       </c>
       <c r="E287" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F287" t="s">
         <v>759</v>
-      </c>
-      <c r="F287" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="288" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -8527,10 +8527,10 @@
         <v>686</v>
       </c>
       <c r="E288" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F288" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="289" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -8603,10 +8603,10 @@
         <v>691</v>
       </c>
       <c r="E293" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F293" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -8679,10 +8679,10 @@
         <v>433</v>
       </c>
       <c r="E298" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F298" t="s">
         <v>759</v>
-      </c>
-      <c r="F298" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="299" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -8699,10 +8699,10 @@
         <v>696</v>
       </c>
       <c r="E299" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="F299" s="3" t="s">
         <v>840</v>
-      </c>
-      <c r="F299" s="3" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="300" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8719,10 +8719,10 @@
         <v>697</v>
       </c>
       <c r="E300" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F300" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="301" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8739,10 +8739,10 @@
         <v>698</v>
       </c>
       <c r="E301" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F301" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8759,10 +8759,10 @@
         <v>699</v>
       </c>
       <c r="E302" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F302" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="303" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -8779,10 +8779,10 @@
         <v>700</v>
       </c>
       <c r="E303" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F303" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="304" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -8799,10 +8799,10 @@
         <v>702</v>
       </c>
       <c r="E304" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="F304" s="3" t="s">
         <v>843</v>
-      </c>
-      <c r="F304" s="3" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.3">
@@ -8819,10 +8819,10 @@
         <v>701</v>
       </c>
       <c r="E305" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F305" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="306" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -8839,10 +8839,10 @@
         <v>703</v>
       </c>
       <c r="E306" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="F306" s="3" t="s">
         <v>843</v>
-      </c>
-      <c r="F306" s="3" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.3">
@@ -8859,10 +8859,10 @@
         <v>704</v>
       </c>
       <c r="E307" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="F307" s="3" t="s">
         <v>843</v>
-      </c>
-      <c r="F307" s="3" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="308" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -8879,10 +8879,10 @@
         <v>705</v>
       </c>
       <c r="E308" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="F308" s="3" t="s">
         <v>843</v>
-      </c>
-      <c r="F308" s="3" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="309" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -8899,10 +8899,10 @@
         <v>706</v>
       </c>
       <c r="E309" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="F309" s="3" t="s">
         <v>843</v>
-      </c>
-      <c r="F309" s="3" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.3">
@@ -8919,10 +8919,10 @@
         <v>433</v>
       </c>
       <c r="E310" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F310" t="s">
         <v>759</v>
-      </c>
-      <c r="F310" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="311" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -8942,7 +8942,7 @@
         <v>755</v>
       </c>
       <c r="F311" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -8962,7 +8962,7 @@
         <v>755</v>
       </c>
       <c r="F312" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="313" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -8982,7 +8982,7 @@
         <v>755</v>
       </c>
       <c r="F313" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -9002,7 +9002,7 @@
         <v>755</v>
       </c>
       <c r="F314" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="315" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -9022,7 +9022,7 @@
         <v>755</v>
       </c>
       <c r="F315" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="316" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -9042,7 +9042,7 @@
         <v>755</v>
       </c>
       <c r="F316" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="317" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -9062,7 +9062,7 @@
         <v>755</v>
       </c>
       <c r="F317" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="318" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -9082,7 +9082,7 @@
         <v>755</v>
       </c>
       <c r="F318" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.3">
@@ -9099,10 +9099,10 @@
         <v>433</v>
       </c>
       <c r="E319" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F319" t="s">
         <v>759</v>
-      </c>
-      <c r="F319" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="320" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9119,7 +9119,7 @@
         <v>717</v>
       </c>
       <c r="E320" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F320">
         <v>1</v>
@@ -9139,7 +9139,7 @@
         <v>716</v>
       </c>
       <c r="E321" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F321">
         <v>1</v>
@@ -9159,7 +9159,7 @@
         <v>718</v>
       </c>
       <c r="E322" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F322">
         <v>1</v>
@@ -9179,7 +9179,7 @@
         <v>719</v>
       </c>
       <c r="E323" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F323">
         <v>1</v>
@@ -9199,10 +9199,10 @@
         <v>556</v>
       </c>
       <c r="E324" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F324" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="325" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9247,10 +9247,10 @@
         <v>556</v>
       </c>
       <c r="E327" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F327" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="328" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9284,7 +9284,7 @@
         <v>755</v>
       </c>
       <c r="F329" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="330" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -9301,10 +9301,10 @@
         <v>556</v>
       </c>
       <c r="E330" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F330" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="331" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -9338,7 +9338,7 @@
         <v>755</v>
       </c>
       <c r="F332" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.3">
@@ -9355,10 +9355,10 @@
         <v>433</v>
       </c>
       <c r="E333" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F333" t="s">
         <v>759</v>
-      </c>
-      <c r="F333" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="334" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -9375,10 +9375,10 @@
         <v>556</v>
       </c>
       <c r="E334" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F334" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="335" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -9395,10 +9395,10 @@
         <v>732</v>
       </c>
       <c r="E335" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F335" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.3">
@@ -9435,7 +9435,7 @@
         <v>735</v>
       </c>
       <c r="E337" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F337">
         <v>1</v>
@@ -9455,7 +9455,7 @@
         <v>736</v>
       </c>
       <c r="E338" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F338">
         <v>1</v>
@@ -9475,7 +9475,7 @@
         <v>737</v>
       </c>
       <c r="E339" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F339">
         <v>1</v>
@@ -9495,10 +9495,10 @@
         <v>556</v>
       </c>
       <c r="E340" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F340" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="341" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9543,10 +9543,10 @@
         <v>556</v>
       </c>
       <c r="E343" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F343" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="344" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -9557,16 +9557,16 @@
         <v>342</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D344" s="3" t="s">
         <v>556</v>
       </c>
       <c r="E344" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F344" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="345" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -9577,7 +9577,7 @@
         <v>343</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D345" s="3" t="s">
         <v>739</v>
@@ -9591,7 +9591,7 @@
         <v>344</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D346" s="3" t="s">
         <v>740</v>
@@ -9611,10 +9611,10 @@
         <v>556</v>
       </c>
       <c r="E347" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F347" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="348" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9659,10 +9659,10 @@
         <v>556</v>
       </c>
       <c r="E350" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F350" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="351" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9707,10 +9707,10 @@
         <v>433</v>
       </c>
       <c r="E353" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F353" t="s">
         <v>759</v>
-      </c>
-      <c r="F353" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="354" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9727,10 +9727,10 @@
         <v>744</v>
       </c>
       <c r="E354" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F354" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="355" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9747,10 +9747,10 @@
         <v>745</v>
       </c>
       <c r="E355" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F355" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="356" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9767,10 +9767,10 @@
         <v>746</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F356" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="357" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -9787,10 +9787,10 @@
         <v>747</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F357" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.3">
@@ -9807,10 +9807,10 @@
         <v>433</v>
       </c>
       <c r="E358" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F358" t="s">
         <v>759</v>
-      </c>
-      <c r="F358" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.3">
@@ -9827,10 +9827,10 @@
         <v>433</v>
       </c>
       <c r="E359" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F359" t="s">
         <v>759</v>
-      </c>
-      <c r="F359" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="360" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -9847,10 +9847,10 @@
         <v>505</v>
       </c>
       <c r="E360" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F360" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F360" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="361" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -9867,10 +9867,10 @@
         <v>506</v>
       </c>
       <c r="E361" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F361" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F361" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="362" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -9887,10 +9887,10 @@
         <v>507</v>
       </c>
       <c r="E362" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F362" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F362" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="363" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -9907,10 +9907,10 @@
         <v>510</v>
       </c>
       <c r="E363" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F363" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F363" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="364" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -9927,10 +9927,10 @@
         <v>511</v>
       </c>
       <c r="E364" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F364" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F364" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="365" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -9947,10 +9947,10 @@
         <v>513</v>
       </c>
       <c r="E365" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F365" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F365" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="366" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -9967,10 +9967,10 @@
         <v>515</v>
       </c>
       <c r="E366" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F366" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="F366" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.3">
@@ -9987,10 +9987,10 @@
         <v>433</v>
       </c>
       <c r="E367" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="F367" t="s">
         <v>759</v>
-      </c>
-      <c r="F367" t="s">
-        <v>760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functions to store question options and implement cell validation
</commit_message>
<xml_diff>
--- a/data/fff-question-lookup.xlsx
+++ b/data/fff-question-lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/FFF-RedCap/FFF-RedCap-data-processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1157" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58032DFA-C0C7-4CBF-BF57-D8E6476E65A6}"/>
+  <xr:revisionPtr revIDLastSave="1163" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FFF040B-8714-4CA2-9C79-2AF5025FA9F7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5520" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2978,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F367"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Imputing data access group
</commit_message>
<xml_diff>
--- a/data/fff-question-lookup.xlsx
+++ b/data/fff-question-lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/FFF-RedCap/FFF-RedCap-data-processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1307" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA1CD19-480B-4F34-AB07-10BE408BD9C0}"/>
+  <xr:revisionPtr revIDLastSave="1309" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E933354B-7E39-4C3C-935E-C06D1BC963EA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-5520" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="857">
   <si>
     <t>record_id</t>
   </si>
@@ -2638,6 +2638,9 @@
   </si>
   <si>
     <t>4. I agree to be part of the evaluation as detailed in the participant information sheet. (Please enter initials)</t>
+  </si>
+  <si>
+    <t>Data Access Group</t>
   </si>
 </sst>
 </file>
@@ -3012,7 +3015,7 @@
   <dimension ref="A1:F367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3083,6 +3086,12 @@
       <c r="C4" s="3" t="s">
         <v>734</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Fixed question lookup loading bug
</commit_message>
<xml_diff>
--- a/data/fff-question-lookup.xlsx
+++ b/data/fff-question-lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/FFF-RedCap/FFF-RedCap-data-processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1309" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E933354B-7E39-4C3C-935E-C06D1BC963EA}"/>
+  <xr:revisionPtr revIDLastSave="1310" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFD88CFD-88D7-4BB5-AAFF-224C2291E3D9}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-5520" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="857">
   <si>
     <t>record_id</t>
   </si>
@@ -3015,7 +3015,7 @@
   <dimension ref="A1:F367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3075,6 +3075,9 @@
       <c r="C3" s="3" t="s">
         <v>734</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Added death literacy questions
</commit_message>
<xml_diff>
--- a/data/fff-question-lookup.xlsx
+++ b/data/fff-question-lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/FFF-RedCap/FFF-RedCap-data-processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1328" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B97454D-AEB4-4096-80F5-6714C8D5D1C5}"/>
+  <xr:revisionPtr revIDLastSave="1424" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41641825-71D7-466B-AC44-47290B1BCC51}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5520" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="937">
   <si>
     <t>record_id</t>
   </si>
@@ -2620,6 +2620,267 @@
   </si>
   <si>
     <t xml:space="preserve">1; </t>
+  </si>
+  <si>
+    <t>death_literacy_index</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q1</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q2</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q3</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q4</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q5</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q6</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q7</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q8</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q9</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q10</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q11</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q12</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q13</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q14</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q15</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q16</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q17</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q18</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q19</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q20</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q21</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q22</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q23</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q24</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q25</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q26</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q27</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q28</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q29</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q30</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q31</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q32</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q33</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q34</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q35</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q36</t>
+  </si>
+  <si>
+    <t>death_literacy_index_q37</t>
+  </si>
+  <si>
+    <t>death_literacy_index_complete</t>
+  </si>
+  <si>
+    <t>Some groups of people report a poorer experience of palliative, end of life care and bereavement support than others therefore we are asking for demographic information to look at any patterns in Birmingham.</t>
+  </si>
+  <si>
+    <t>TOPIC: Support groups in my community I am aware of support in my community for…</t>
+  </si>
+  <si>
+    <t>Is there anything you would like to tell us about your experiences in Birmingham that is relevant to this survey?</t>
+  </si>
+  <si>
+    <t>COMMUNITY KNOWLEDGE TOPIC: Others can help me provide end of life care Please rate your level of agreement with the following statements - If I were toprovide end of life care for someone, I know people who could help me:</t>
+  </si>
+  <si>
+    <t>WHAT YOU KNOW TOPIC: Knowledge of what to do around end-of-life care</t>
+  </si>
+  <si>
+    <t>YOUR EXPERIENCES TOPIC - Grief and loss Please rate your level of agreement with the following statements. Indicate your response on a scale where 1 = do not agree at all to 5 = strongly agree My previous experience of grief, loss or other significant life events has:</t>
+  </si>
+  <si>
+    <t>TOPIC - Providing hands on care Would you be able to do the following</t>
+  </si>
+  <si>
+    <t>Death Literacy Index *The Death Literacy Questionnaire* was developed in order to help understand a communities' strengths on issues relating to death, dying and loss. It also highlights opportunities for additional community skills enhancement. Responses to the survey are anonymous and no sensitive data is required or stored. This version has been adapted by Compassionate Birmingham to meet Plain English written standards. The meaning of the questions remain as per the original. If there is a question that you do not know the answer to, answer as best as you can based on what you think you would know/do in that situation. *Leonard, R., Noonan, K., Horsfall, D., Psychogios, H., Kelly, M., Rosenberg, J., Rumbold, B., Grindrod, A., Read, N., and Rahn, A. (2020). Death Literacy Index: A Report on its Development and Implementation. Sydney: Western Sydney University. https://doi.org/10.26183/5eb8d3adb20b0 PRACTICAL KNOWLEDGE TOPIC -Conversations about dying, death and grief Please rate your level of confidence with the following statements. Indicate your response on a scale where 1 = not at all able to5 = very able</t>
+  </si>
+  <si>
+    <t>1. Talking about death, dying and grief to a close friend</t>
+  </si>
+  <si>
+    <t>2. Talking about death, dying and grief to a child</t>
+  </si>
+  <si>
+    <t>3. Talking to a grieving person about their loss</t>
+  </si>
+  <si>
+    <t>4. Talking to a GP about getting support for a dying person</t>
+  </si>
+  <si>
+    <t>5. Feed or help a person to eat</t>
+  </si>
+  <si>
+    <t>6. Bath a person</t>
+  </si>
+  <si>
+    <t>7. Lift a person or help them move</t>
+  </si>
+  <si>
+    <t>8. Give injections</t>
+  </si>
+  <si>
+    <t>10. Made me think about what is important and not important in life</t>
+  </si>
+  <si>
+    <t>11. Developed my wisdom and understanding</t>
+  </si>
+  <si>
+    <t>12. Made me kinder and more compassionate toward myself</t>
+  </si>
+  <si>
+    <t>13. Made me better prepared to face similar challenges in the future</t>
+  </si>
+  <si>
+    <t>14. I know the rules and regulations for when a person dies at home</t>
+  </si>
+  <si>
+    <t>15. I know what documents are needed when planning forsomeone's death</t>
+  </si>
+  <si>
+    <t>16. I know enough about the healthcare system to find the support that a dying person needs</t>
+  </si>
+  <si>
+    <t>17. I know enough to make decisions about different types of funeral arrangements</t>
+  </si>
+  <si>
+    <t>9. Made me more emotionally prepared to support others with death, dying and bereavement</t>
+  </si>
+  <si>
+    <t>18. I know how to access palliative care in my area [palliative care is where a team of healthcare professionals support someone who is seriously ill in their physical, psychological, social and spiritual health]</t>
+  </si>
+  <si>
+    <t>19. I know enough about how different illnesses progress to make choices about medical treatments towards the end of life</t>
+  </si>
+  <si>
+    <t>20. I know how funeral directors can help</t>
+  </si>
+  <si>
+    <t>21. to get support in the area where I live, e.g. from clubs, support groups, associations, or volunteer organisations</t>
+  </si>
+  <si>
+    <t>22. to get help with providing day-to-day care for a person at the end of life</t>
+  </si>
+  <si>
+    <t>23. to get equipment that is needed to help care for someone</t>
+  </si>
+  <si>
+    <t>24. to get support that is culturally appropriate for a person</t>
+  </si>
+  <si>
+    <t>25. to get emotional support for myself</t>
+  </si>
+  <si>
+    <t>26. people with life threatening illnesses</t>
+  </si>
+  <si>
+    <t>27. people who are nearing the end of their life</t>
+  </si>
+  <si>
+    <t>28. people who are caring for a dying person</t>
+  </si>
+  <si>
+    <t>29. people who are grieving</t>
+  </si>
+  <si>
+    <t>30. What are the first 3 letters/numbers of your postcode</t>
+  </si>
+  <si>
+    <t>31. How old are you?</t>
+  </si>
+  <si>
+    <t>32. How would you describe your ethnicity?</t>
+  </si>
+  <si>
+    <t>33. How would you define your gender?</t>
+  </si>
+  <si>
+    <t>34. How would you describe your sexuality?</t>
+  </si>
+  <si>
+    <t>35. Do you work in a health or care role?</t>
+  </si>
+  <si>
+    <t>36. Have you ever cared for someone who was dying?</t>
+  </si>
+  <si>
+    <t>37. Is there anything you would like to tell us about your experiences in Birmingham that is relevant to this survey?</t>
+  </si>
+  <si>
+    <t>1 - Not able; 2, 3, 4, 5 - Very able</t>
+  </si>
+  <si>
+    <t>1 - do not agree at all; 2; 3; 4; 5 - strongly agree</t>
+  </si>
+  <si>
+    <t>Under 18; 18-24; 25-34; 35-44; 45-54; 55-64; 65+</t>
   </si>
 </sst>
 </file>
@@ -2991,15 +3252,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F360"/>
+  <dimension ref="A1:F398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="D391" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E398" sqref="E398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="1" max="1" width="45.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" customWidth="1"/>
     <col min="3" max="3" width="43.21875" style="3" customWidth="1"/>
     <col min="4" max="4" width="67.44140625" style="3" customWidth="1"/>
@@ -9921,6 +10182,736 @@
         <v>729</v>
       </c>
     </row>
+    <row r="361" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>850</v>
+      </c>
+      <c r="B361" t="s">
+        <v>851</v>
+      </c>
+      <c r="C361" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="D361" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="E361" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F361" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>850</v>
+      </c>
+      <c r="B362" t="s">
+        <v>852</v>
+      </c>
+      <c r="C362" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="D362" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="E362" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F362" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>850</v>
+      </c>
+      <c r="B363" t="s">
+        <v>853</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="D363" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="E363" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F363" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>850</v>
+      </c>
+      <c r="B364" t="s">
+        <v>854</v>
+      </c>
+      <c r="C364" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="D364" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="E364" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F364" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>850</v>
+      </c>
+      <c r="B365" t="s">
+        <v>855</v>
+      </c>
+      <c r="C365" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="D365" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="E365" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F365" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>850</v>
+      </c>
+      <c r="B366" t="s">
+        <v>856</v>
+      </c>
+      <c r="C366" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="D366" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="E366" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F366" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>850</v>
+      </c>
+      <c r="B367" t="s">
+        <v>857</v>
+      </c>
+      <c r="C367" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="D367" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="E367" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F367" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>850</v>
+      </c>
+      <c r="B368" t="s">
+        <v>858</v>
+      </c>
+      <c r="C368" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="D368" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="E368" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F368" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>850</v>
+      </c>
+      <c r="B369" t="s">
+        <v>859</v>
+      </c>
+      <c r="C369" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="D369" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="E369" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F369" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>850</v>
+      </c>
+      <c r="B370" t="s">
+        <v>860</v>
+      </c>
+      <c r="C370" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="D370" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="E370" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F370" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>850</v>
+      </c>
+      <c r="B371" t="s">
+        <v>861</v>
+      </c>
+      <c r="C371" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="D371" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="E371" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F371" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>850</v>
+      </c>
+      <c r="B372" t="s">
+        <v>862</v>
+      </c>
+      <c r="C372" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="D372" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="E372" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F372" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A373" t="s">
+        <v>850</v>
+      </c>
+      <c r="B373" t="s">
+        <v>863</v>
+      </c>
+      <c r="C373" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="D373" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="E373" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F373" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>850</v>
+      </c>
+      <c r="B374" t="s">
+        <v>864</v>
+      </c>
+      <c r="C374" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="D374" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="E374" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F374" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>850</v>
+      </c>
+      <c r="B375" t="s">
+        <v>865</v>
+      </c>
+      <c r="C375" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="D375" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="E375" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F375" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>850</v>
+      </c>
+      <c r="B376" t="s">
+        <v>866</v>
+      </c>
+      <c r="C376" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="D376" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="E376" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F376" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A377" t="s">
+        <v>850</v>
+      </c>
+      <c r="B377" t="s">
+        <v>867</v>
+      </c>
+      <c r="C377" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="D377" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="E377" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F377" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A378" t="s">
+        <v>850</v>
+      </c>
+      <c r="B378" t="s">
+        <v>868</v>
+      </c>
+      <c r="C378" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="D378" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F378" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A379" t="s">
+        <v>850</v>
+      </c>
+      <c r="B379" t="s">
+        <v>869</v>
+      </c>
+      <c r="C379" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="D379" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="E379" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F379" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>850</v>
+      </c>
+      <c r="B380" t="s">
+        <v>870</v>
+      </c>
+      <c r="C380" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="D380" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F380" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>850</v>
+      </c>
+      <c r="B381" t="s">
+        <v>871</v>
+      </c>
+      <c r="C381" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="D381" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="E381" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F381" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>850</v>
+      </c>
+      <c r="B382" t="s">
+        <v>872</v>
+      </c>
+      <c r="C382" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="D382" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F382" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>850</v>
+      </c>
+      <c r="B383" t="s">
+        <v>873</v>
+      </c>
+      <c r="C383" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="D383" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="E383" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F383" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>850</v>
+      </c>
+      <c r="B384" t="s">
+        <v>874</v>
+      </c>
+      <c r="C384" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="D384" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="E384" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F384" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>850</v>
+      </c>
+      <c r="B385" t="s">
+        <v>875</v>
+      </c>
+      <c r="C385" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="D385" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="E385" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F385" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>850</v>
+      </c>
+      <c r="B386" t="s">
+        <v>876</v>
+      </c>
+      <c r="C386" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="D386" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F386" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>850</v>
+      </c>
+      <c r="B387" t="s">
+        <v>877</v>
+      </c>
+      <c r="C387" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="D387" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="E387" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F387" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>850</v>
+      </c>
+      <c r="B388" t="s">
+        <v>878</v>
+      </c>
+      <c r="C388" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="D388" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F388" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>850</v>
+      </c>
+      <c r="B389" t="s">
+        <v>879</v>
+      </c>
+      <c r="C389" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="D389" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="E389" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F389" s="8" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>850</v>
+      </c>
+      <c r="B390" t="s">
+        <v>880</v>
+      </c>
+      <c r="C390" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="D390" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A391" t="s">
+        <v>850</v>
+      </c>
+      <c r="B391" t="s">
+        <v>881</v>
+      </c>
+      <c r="C391" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="D391" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="E391" s="5" t="s">
+        <v>936</v>
+      </c>
+      <c r="F391" s="8" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>850</v>
+      </c>
+      <c r="B392" t="s">
+        <v>882</v>
+      </c>
+      <c r="C392" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="D392" s="3" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>850</v>
+      </c>
+      <c r="B393" t="s">
+        <v>883</v>
+      </c>
+      <c r="C393" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="D393" s="3" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>850</v>
+      </c>
+      <c r="B394" t="s">
+        <v>884</v>
+      </c>
+      <c r="C394" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="D394" s="3" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A395" t="s">
+        <v>850</v>
+      </c>
+      <c r="B395" t="s">
+        <v>885</v>
+      </c>
+      <c r="C395" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="D395" s="3" t="s">
+        <v>931</v>
+      </c>
+      <c r="E395" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F395" s="8" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A396" t="s">
+        <v>850</v>
+      </c>
+      <c r="B396" t="s">
+        <v>886</v>
+      </c>
+      <c r="C396" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="D396" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="E396" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F396" s="8" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>850</v>
+      </c>
+      <c r="B397" t="s">
+        <v>887</v>
+      </c>
+      <c r="C397" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="D397" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="E397" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="F397" s="8" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>850</v>
+      </c>
+      <c r="B398" t="s">
+        <v>888</v>
+      </c>
+      <c r="C398" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D398" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Lubben Social Network questions to lookup
</commit_message>
<xml_diff>
--- a/data/fff-question-lookup.xlsx
+++ b/data/fff-question-lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/FFF-RedCap/FFF-RedCap-data-processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1424" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41641825-71D7-466B-AC44-47290B1BCC51}"/>
+  <xr:revisionPtr revIDLastSave="1491" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E487AB1D-31C0-48AF-A970-71F18E46E4C5}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="983">
   <si>
     <t>record_id</t>
   </si>
@@ -2881,6 +2881,144 @@
   </si>
   <si>
     <t>Under 18; 18-24; 25-34; 35-44; 45-54; 55-64; 65+</t>
+  </si>
+  <si>
+    <t>lubben_social_network_scale_revised_lsnsr</t>
+  </si>
+  <si>
+    <t>lsns_r_q1</t>
+  </si>
+  <si>
+    <t>lsns_r_q2</t>
+  </si>
+  <si>
+    <t>lsns_r_q3</t>
+  </si>
+  <si>
+    <t>lsns_r_q4</t>
+  </si>
+  <si>
+    <t>lsns_r_q5</t>
+  </si>
+  <si>
+    <t>lsns_r_q6</t>
+  </si>
+  <si>
+    <t>lsns_r_q7</t>
+  </si>
+  <si>
+    <t>lsns_r_q8</t>
+  </si>
+  <si>
+    <t>lsns_r_q9</t>
+  </si>
+  <si>
+    <t>lsns_r_q10</t>
+  </si>
+  <si>
+    <t>lsns_r_q11</t>
+  </si>
+  <si>
+    <t>lsns_r_q12</t>
+  </si>
+  <si>
+    <t>lubben_social_network_scale_revised_lsnsr_complete</t>
+  </si>
+  <si>
+    <t>LUBBEN SOCIAL NETWORK SCALE - REVISED (LSNS-R) FAMILY: Considering the people to whom you are related by birth, marriage, adoption, etc…</t>
+  </si>
+  <si>
+    <t>FRIENDSHIPS: Considering all of your friends including those who live in your neighbourhood...</t>
+  </si>
+  <si>
+    <t>1. How many relatives do you see or hear from at least once a month?</t>
+  </si>
+  <si>
+    <t>2. How often do you see or hear from the relative with whom you have the most contact?</t>
+  </si>
+  <si>
+    <t>3. How many relatives do you feel at ease with that you can talk about private matters?</t>
+  </si>
+  <si>
+    <t>4. How many relatives do you feel close to such that you could call on them for help?</t>
+  </si>
+  <si>
+    <t>5. When one of your relatives has an important decision to make, how often do they talk to you about it?</t>
+  </si>
+  <si>
+    <t>6. How often is one of your relatives available for you to talk to when you have an important decision to make?</t>
+  </si>
+  <si>
+    <t>7. How many of your friends do you see or hear from at least once a month?</t>
+  </si>
+  <si>
+    <t>8. How often do you see or hear from the friend with whom you have the most contact?</t>
+  </si>
+  <si>
+    <t>9. How many friends do you feel at ease with that you can talk about private matters?</t>
+  </si>
+  <si>
+    <t>10. How many friends do you feel close to such that you could call on them for help?</t>
+  </si>
+  <si>
+    <t>11. When one of your friends has an important decision to make, how often do they talk to you about it?</t>
+  </si>
+  <si>
+    <t>12. How often is one of your friends available for you to talk to when you have an important decision to make?</t>
+  </si>
+  <si>
+    <t>0 = none; 1 = one; 2 = two; 3 = three or four; 4 = five thru eight; 5 = nine or more</t>
+  </si>
+  <si>
+    <t>0; 1; 2; 3; 4; 5</t>
+  </si>
+  <si>
+    <t>0 = less than monthly; 1 = monthly; 2 = few times a month; 3 = weekly; 4 = few times a week; 5 = daily</t>
+  </si>
+  <si>
+    <t>0 = never; 1 = seldom; 2 = sometimes; 3 = often; 4 = very often; 5 = always</t>
+  </si>
+  <si>
+    <t>lubben_social_network_scale_6_lsns_6</t>
+  </si>
+  <si>
+    <t>lsns_6_q1</t>
+  </si>
+  <si>
+    <t>lsns_6_q2</t>
+  </si>
+  <si>
+    <t>lsns_6_q3</t>
+  </si>
+  <si>
+    <t>lsns_6_q4</t>
+  </si>
+  <si>
+    <t>lsns_6_q5</t>
+  </si>
+  <si>
+    <t>lsns_6_q6</t>
+  </si>
+  <si>
+    <t>LUBBEN SOCIAL NETWORK SCALE - REVISED (LSNS-R) FAMILY: Considering the people to whom you are related by birth, marriage, adoption, etc...</t>
+  </si>
+  <si>
+    <t>2. How many relatives do you feel at ease with that you can talk about private matters?</t>
+  </si>
+  <si>
+    <t>3. How many relatives do you feel close to such that you could call on them for help?</t>
+  </si>
+  <si>
+    <t>4. How many of your friends do you see or hear from at least once a month?</t>
+  </si>
+  <si>
+    <t>5. How many friends do you feel at ease with that you can talk about private matters?</t>
+  </si>
+  <si>
+    <t>6. How many friends do you feel close to such that you could call on them for help?</t>
+  </si>
+  <si>
+    <t>lubben_social_network_scale_6_lsns_6_complete</t>
   </si>
 </sst>
 </file>
@@ -3252,10 +3390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F398"/>
+  <dimension ref="A1:F418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D391" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E398" sqref="E398"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10912,6 +11050,406 @@
         <v>423</v>
       </c>
     </row>
+    <row r="399" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>937</v>
+      </c>
+      <c r="B399" t="s">
+        <v>938</v>
+      </c>
+      <c r="C399" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="D399" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="E399" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F399" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>937</v>
+      </c>
+      <c r="B400" t="s">
+        <v>939</v>
+      </c>
+      <c r="C400" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="D400" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="E400" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="F400" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A401" t="s">
+        <v>937</v>
+      </c>
+      <c r="B401" t="s">
+        <v>940</v>
+      </c>
+      <c r="C401" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="D401" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="E401" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F401" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A402" t="s">
+        <v>937</v>
+      </c>
+      <c r="B402" t="s">
+        <v>941</v>
+      </c>
+      <c r="C402" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="D402" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="E402" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F402" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>937</v>
+      </c>
+      <c r="B403" t="s">
+        <v>942</v>
+      </c>
+      <c r="C403" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="D403" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="E403" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="F403" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>937</v>
+      </c>
+      <c r="B404" t="s">
+        <v>943</v>
+      </c>
+      <c r="C404" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="D404" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="E404" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="F404" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A405" t="s">
+        <v>937</v>
+      </c>
+      <c r="B405" t="s">
+        <v>944</v>
+      </c>
+      <c r="C405" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D405" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="E405" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F405" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>937</v>
+      </c>
+      <c r="B406" t="s">
+        <v>945</v>
+      </c>
+      <c r="C406" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D406" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="E406" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="F406" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A407" t="s">
+        <v>937</v>
+      </c>
+      <c r="B407" t="s">
+        <v>946</v>
+      </c>
+      <c r="C407" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D407" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="E407" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F407" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A408" t="s">
+        <v>937</v>
+      </c>
+      <c r="B408" t="s">
+        <v>947</v>
+      </c>
+      <c r="C408" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D408" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="E408" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F408" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A409" t="s">
+        <v>937</v>
+      </c>
+      <c r="B409" t="s">
+        <v>948</v>
+      </c>
+      <c r="C409" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D409" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="E409" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="F409" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A410" t="s">
+        <v>937</v>
+      </c>
+      <c r="B410" t="s">
+        <v>949</v>
+      </c>
+      <c r="C410" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D410" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="E410" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="F410" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>937</v>
+      </c>
+      <c r="B411" t="s">
+        <v>950</v>
+      </c>
+      <c r="C411" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D411" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E411" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="F411" s="8" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>969</v>
+      </c>
+      <c r="B412" t="s">
+        <v>970</v>
+      </c>
+      <c r="C412" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="D412" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="E412" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F412" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>969</v>
+      </c>
+      <c r="B413" t="s">
+        <v>971</v>
+      </c>
+      <c r="C413" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="D413" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="E413" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F413" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>969</v>
+      </c>
+      <c r="B414" t="s">
+        <v>972</v>
+      </c>
+      <c r="C414" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="D414" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="E414" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F414" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>969</v>
+      </c>
+      <c r="B415" t="s">
+        <v>973</v>
+      </c>
+      <c r="C415" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D415" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="E415" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F415" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>969</v>
+      </c>
+      <c r="B416" t="s">
+        <v>974</v>
+      </c>
+      <c r="C416" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D416" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E416" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F416" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>969</v>
+      </c>
+      <c r="B417" t="s">
+        <v>975</v>
+      </c>
+      <c r="C417" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="D417" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="E417" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F417" s="8" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>969</v>
+      </c>
+      <c r="B418" t="s">
+        <v>982</v>
+      </c>
+      <c r="C418" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D418" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E418" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="F418" s="8" t="s">
+        <v>729</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added health promotion and asthma qs
</commit_message>
<xml_diff>
--- a/data/fff-question-lookup.xlsx
+++ b/data/fff-question-lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/FFF-RedCap/FFF-RedCap-data-processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1491" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E487AB1D-31C0-48AF-A970-71F18E46E4C5}"/>
+  <xr:revisionPtr revIDLastSave="1607" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F629EB83-3C60-47F6-9A12-16F32CC3C898}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2548" uniqueCount="1039">
   <si>
     <t>record_id</t>
   </si>
@@ -3019,6 +3019,174 @@
   </si>
   <si>
     <t>lubben_social_network_scale_6_lsns_6_complete</t>
+  </si>
+  <si>
+    <t>asthma_and_home_safety_survey</t>
+  </si>
+  <si>
+    <t>asthma_pre_question_1</t>
+  </si>
+  <si>
+    <t>asthma_pre_question_2</t>
+  </si>
+  <si>
+    <t>asthma_pre_question_3</t>
+  </si>
+  <si>
+    <t>asthma_pre_question_4</t>
+  </si>
+  <si>
+    <t>asthma_pre_question_4a</t>
+  </si>
+  <si>
+    <t>asthma_post_question_1</t>
+  </si>
+  <si>
+    <t>asthma_post_question_2</t>
+  </si>
+  <si>
+    <t>asthma_post_question_3</t>
+  </si>
+  <si>
+    <t>asthma_post_question_4</t>
+  </si>
+  <si>
+    <t>asthma_post_question_4a</t>
+  </si>
+  <si>
+    <t>asthma_fu_question_1</t>
+  </si>
+  <si>
+    <t>asthma_fu_question_1a</t>
+  </si>
+  <si>
+    <t>asthma_fu_question_2</t>
+  </si>
+  <si>
+    <t>asthma_fu_question_3</t>
+  </si>
+  <si>
+    <t>asthma_fu_question_4</t>
+  </si>
+  <si>
+    <t>asthma_and_home_safety_survey_complete</t>
+  </si>
+  <si>
+    <t>Asthma and Home Safety Survey - Pre-Intervention Questionnaire. Please answer the following questions based on: 1 = Not confident5 = Very confident</t>
+  </si>
+  <si>
+    <t>Asthma and Home Safety Survey - Post-Intervention Questionnaire. Please answer the following questions based on: 1 = Not confident5 = Very confident</t>
+  </si>
+  <si>
+    <t>Asthma and Home Safety Survey - Follow-Up Questionnaire. Please answer the following questions based on: 1 = Not confident, 5 = Very confident</t>
+  </si>
+  <si>
+    <t>1. On a scale of 1 to 5, how confident do you feel recognising the signs of an asthma attack?</t>
+  </si>
+  <si>
+    <t>2. On a scale of 1 to 5, how confident do you feel about using an asthma inhaler and spacer correctly?</t>
+  </si>
+  <si>
+    <t>3. On a scale of 1 to 5, how safe do you feel your home is for young children?</t>
+  </si>
+  <si>
+    <t>4. Have you or your child ever been admitted to hospital due to asthma or a home accident?</t>
+  </si>
+  <si>
+    <t>Please give a brief description:Optional</t>
+  </si>
+  <si>
+    <t>Please give a brief description: Optional</t>
+  </si>
+  <si>
+    <t>1 - Not confident; 2; 3; 4; 5 - Very confident</t>
+  </si>
+  <si>
+    <t>4. Have you made (or do you plan to make) any changes at home or in asthma management because of what you learned?</t>
+  </si>
+  <si>
+    <t>1. Since attending, have you used anything you learned to helpmanage asthma or improve safety at home?</t>
+  </si>
+  <si>
+    <t>4. Have you or your child had any asthma-related or injury-related hospital visits since taking part?</t>
+  </si>
+  <si>
+    <t>3. On a scale of 1 to 5, how safe would you rate your home now,c ompared to before the programme?</t>
+  </si>
+  <si>
+    <t>2. On a scale of 1 to 5, how confident do you now feel handling an asthma emergency?</t>
+  </si>
+  <si>
+    <t>health_promotion_survey</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q1</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q2</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q2_other</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q3</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q4</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q4a</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q4b</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q4c</t>
+  </si>
+  <si>
+    <t>health_prom_survey_q4d</t>
+  </si>
+  <si>
+    <t>health_promotion_survey_complete</t>
+  </si>
+  <si>
+    <t>1. What was the nature of the event?</t>
+  </si>
+  <si>
+    <t>2. What was the event about?</t>
+  </si>
+  <si>
+    <t>2. What was the event about? - Other</t>
+  </si>
+  <si>
+    <t>3. How was the event delivered?</t>
+  </si>
+  <si>
+    <t>My trust in health care services has increased</t>
+  </si>
+  <si>
+    <t>I have a better understanding of where to go for advice &amp; support</t>
+  </si>
+  <si>
+    <t>I feel more confident about managing my health</t>
+  </si>
+  <si>
+    <t>Health Promotion Survey</t>
+  </si>
+  <si>
+    <t>Health Promotion; Training; Workshop; Group Discussion</t>
+  </si>
+  <si>
+    <t>Smoking; Obesity/Weight management; Physical Activity; Diet/Nutrition; Screening; Immunisations and Vaccinations; Diabetes; Cardiovascular Health; Asthma/Respiratory Health; Sexual Health; Mental Health; Maintaining Wellbeing; Health Promotion; Behaviour Change (for example motivational interviewing); Understanding Communities; Children and Young People; Adult Health; Healthy Aging; LGBTQ+; Learning Disabilities or Autism; Visual or Hearing Impairment; Maternal Health; Other</t>
+  </si>
+  <si>
+    <t>1; 2; 3; 4; 5; 6; 7; 8; 9; 10; 11; 12; 13; 14; 15; 16; 17; 18; 19; 20; 21; 22; O</t>
+  </si>
+  <si>
+    <t>4. Event Content (describe)</t>
+  </si>
+  <si>
+    <t>Stronly Disagree; Disagree; Neither Agree nor Disagree; Agree; Stronly Agree</t>
   </si>
 </sst>
 </file>
@@ -3088,7 +3256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3106,10 +3274,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3390,10 +3560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F418"/>
+  <dimension ref="A1:F444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView tabSelected="1" topLeftCell="A436" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E437" sqref="E437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3403,7 +3573,7 @@
     <col min="3" max="3" width="43.21875" style="3" customWidth="1"/>
     <col min="4" max="4" width="67.44140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="29.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -3422,7 +3592,7 @@
       <c r="E1" s="6" t="s">
         <v>724</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>820</v>
       </c>
     </row>
@@ -3535,7 +3705,7 @@
       <c r="E8" s="5" t="s">
         <v>726</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>727</v>
       </c>
     </row>
@@ -3597,7 +3767,7 @@
       <c r="E12" s="5" t="s">
         <v>725</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3629,7 +3799,7 @@
       <c r="E14" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -3649,7 +3819,7 @@
       <c r="E15" s="5" t="s">
         <v>726</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>727</v>
       </c>
     </row>
@@ -3669,7 +3839,7 @@
       <c r="E16" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -3835,7 +4005,7 @@
       <c r="E27" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -4774,7 +4944,6 @@
       <c r="D75" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
@@ -5040,7 +5209,7 @@
       <c r="E89" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F89" s="8" t="s">
+      <c r="F89" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -5340,7 +5509,7 @@
       <c r="E104" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F104" s="8" t="s">
+      <c r="F104" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -5600,7 +5769,7 @@
       <c r="E117" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F117" s="8" t="s">
+      <c r="F117" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -5620,7 +5789,7 @@
       <c r="E118" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F118" s="8" t="s">
+      <c r="F118" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5640,7 +5809,7 @@
       <c r="E119" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F119" s="8" t="s">
+      <c r="F119" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5660,7 +5829,7 @@
       <c r="E120" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F120" s="8" t="s">
+      <c r="F120" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5680,7 +5849,7 @@
       <c r="E121" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F121" s="8" t="s">
+      <c r="F121" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5700,7 +5869,7 @@
       <c r="E122" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F122" s="8" t="s">
+      <c r="F122" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5720,7 +5889,7 @@
       <c r="E123" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F123" s="8" t="s">
+      <c r="F123" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5740,7 +5909,7 @@
       <c r="E124" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F124" s="8" t="s">
+      <c r="F124" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5760,7 +5929,7 @@
       <c r="E125" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F125" s="8" t="s">
+      <c r="F125" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5780,7 +5949,7 @@
       <c r="E126" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F126" s="8" t="s">
+      <c r="F126" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5800,7 +5969,7 @@
       <c r="E127" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F127" s="8" t="s">
+      <c r="F127" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5820,7 +5989,7 @@
       <c r="E128" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F128" s="8" t="s">
+      <c r="F128" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5840,7 +6009,7 @@
       <c r="E129" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F129" s="8" t="s">
+      <c r="F129" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5860,7 +6029,7 @@
       <c r="E130" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F130" s="8" t="s">
+      <c r="F130" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5880,7 +6049,7 @@
       <c r="E131" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F131" s="8" t="s">
+      <c r="F131" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5900,7 +6069,7 @@
       <c r="E132" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F132" s="8" t="s">
+      <c r="F132" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5920,7 +6089,7 @@
       <c r="E133" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F133" s="8" t="s">
+      <c r="F133" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5940,7 +6109,7 @@
       <c r="E134" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F134" s="8" t="s">
+      <c r="F134" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5960,7 +6129,7 @@
       <c r="E135" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F135" s="8" t="s">
+      <c r="F135" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -5980,7 +6149,7 @@
       <c r="E136" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F136" s="8" t="s">
+      <c r="F136" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6000,7 +6169,7 @@
       <c r="E137" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F137" s="8" t="s">
+      <c r="F137" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6020,7 +6189,7 @@
       <c r="E138" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F138" s="8" t="s">
+      <c r="F138" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6040,7 +6209,7 @@
       <c r="E139" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F139" s="8" t="s">
+      <c r="F139" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6060,7 +6229,7 @@
       <c r="E140" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F140" s="8" t="s">
+      <c r="F140" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6368,7 +6537,7 @@
       <c r="E156" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F156" s="8" t="s">
+      <c r="F156" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -6428,7 +6597,7 @@
       <c r="E159" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F159" s="8" t="s">
+      <c r="F159" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6448,7 +6617,7 @@
       <c r="E160" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F160" s="8" t="s">
+      <c r="F160" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6468,7 +6637,7 @@
       <c r="E161" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F161" s="8" t="s">
+      <c r="F161" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6488,7 +6657,7 @@
       <c r="E162" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F162" s="8" t="s">
+      <c r="F162" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6508,7 +6677,7 @@
       <c r="E163" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F163" s="8" t="s">
+      <c r="F163" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6528,7 +6697,7 @@
       <c r="E164" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F164" s="8" t="s">
+      <c r="F164" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6548,7 +6717,7 @@
       <c r="E165" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F165" s="8" t="s">
+      <c r="F165" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6588,7 +6757,7 @@
       <c r="E167" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F167" s="8" t="s">
+      <c r="F167" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6608,7 +6777,7 @@
       <c r="E168" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F168" s="8" t="s">
+      <c r="F168" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6628,7 +6797,7 @@
       <c r="E169" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F169" s="8" t="s">
+      <c r="F169" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6648,7 +6817,7 @@
       <c r="E170" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F170" s="8" t="s">
+      <c r="F170" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6668,7 +6837,7 @@
       <c r="E171" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F171" s="8" t="s">
+      <c r="F171" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6688,7 +6857,7 @@
       <c r="E172" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F172" s="8" t="s">
+      <c r="F172" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6708,7 +6877,7 @@
       <c r="E173" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F173" s="8" t="s">
+      <c r="F173" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6728,7 +6897,7 @@
       <c r="E174" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F174" s="8" t="s">
+      <c r="F174" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -7008,7 +7177,7 @@
       <c r="E188" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F188" s="8" t="s">
+      <c r="F188" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -7102,7 +7271,7 @@
       <c r="E193" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F193" s="8" t="s">
+      <c r="F193" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -7442,7 +7611,7 @@
       <c r="E210" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F210" s="8" t="s">
+      <c r="F210" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -7842,7 +8011,7 @@
       <c r="E230" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F230" s="8" t="s">
+      <c r="F230" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -8162,7 +8331,7 @@
       <c r="E246" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F246" s="8" t="s">
+      <c r="F246" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -8222,7 +8391,7 @@
       <c r="E249" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F249" s="8" t="s">
+      <c r="F249" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -8242,7 +8411,7 @@
       <c r="E250" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F250" s="8" t="s">
+      <c r="F250" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -8262,7 +8431,7 @@
       <c r="E251" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F251" s="8" t="s">
+      <c r="F251" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -8282,7 +8451,7 @@
       <c r="E252" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F252" s="8" t="s">
+      <c r="F252" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -8302,7 +8471,7 @@
       <c r="E253" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F253" s="8" t="s">
+      <c r="F253" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -8322,7 +8491,7 @@
       <c r="E254" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F254" s="8" t="s">
+      <c r="F254" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -8342,7 +8511,7 @@
       <c r="E255" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F255" s="8" t="s">
+      <c r="F255" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -8362,7 +8531,7 @@
       <c r="E256" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F256" s="8" t="s">
+      <c r="F256" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -8416,7 +8585,7 @@
       <c r="E259" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F259" s="8" t="s">
+      <c r="F259" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -8530,7 +8699,7 @@
       <c r="E265" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F265" s="8" t="s">
+      <c r="F265" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -8830,7 +8999,7 @@
       <c r="E280" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F280" s="8" t="s">
+      <c r="F280" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -9002,7 +9171,7 @@
       <c r="E291" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F291" s="8" t="s">
+      <c r="F291" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -9242,7 +9411,7 @@
       <c r="E303" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F303" s="8" t="s">
+      <c r="F303" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -9422,7 +9591,7 @@
       <c r="E312" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F312" s="8" t="s">
+      <c r="F312" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -9442,7 +9611,7 @@
       <c r="E313" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="F313" s="8" t="s">
+      <c r="F313" s="5" t="s">
         <v>849</v>
       </c>
     </row>
@@ -9462,7 +9631,7 @@
       <c r="E314" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="F314" s="8" t="s">
+      <c r="F314" s="5" t="s">
         <v>849</v>
       </c>
     </row>
@@ -9482,7 +9651,7 @@
       <c r="E315" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="F315" s="8" t="s">
+      <c r="F315" s="5" t="s">
         <v>849</v>
       </c>
     </row>
@@ -9502,7 +9671,7 @@
       <c r="E316" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="F316" s="8" t="s">
+      <c r="F316" s="5" t="s">
         <v>849</v>
       </c>
     </row>
@@ -9684,7 +9853,7 @@
       <c r="E326" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F326" s="8" t="s">
+      <c r="F326" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -9724,7 +9893,7 @@
       <c r="E328" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="F328" s="8" t="s">
+      <c r="F328" s="5" t="s">
         <v>770</v>
       </c>
     </row>
@@ -9744,7 +9913,7 @@
       <c r="E329" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="F329" s="8" t="s">
+      <c r="F329" s="5" t="s">
         <v>847</v>
       </c>
     </row>
@@ -9764,7 +9933,7 @@
       <c r="E330" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F330" s="8" t="s">
+      <c r="F330" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -9784,7 +9953,7 @@
       <c r="E331" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F331" s="8" t="s">
+      <c r="F331" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -9804,7 +9973,7 @@
       <c r="E332" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="F332" s="8" t="s">
+      <c r="F332" s="5" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10036,7 +10205,7 @@
       <c r="E346" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F346" s="8" t="s">
+      <c r="F346" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -10136,7 +10305,7 @@
       <c r="E351" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F351" s="8" t="s">
+      <c r="F351" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -10156,7 +10325,7 @@
       <c r="E352" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F352" s="8" t="s">
+      <c r="F352" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -10316,7 +10485,7 @@
       <c r="E360" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F360" s="8" t="s">
+      <c r="F360" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -10336,7 +10505,7 @@
       <c r="E361" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F361" s="8" t="s">
+      <c r="F361" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10356,7 +10525,7 @@
       <c r="E362" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F362" s="8" t="s">
+      <c r="F362" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10376,7 +10545,7 @@
       <c r="E363" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F363" s="8" t="s">
+      <c r="F363" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10396,7 +10565,7 @@
       <c r="E364" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F364" s="8" t="s">
+      <c r="F364" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10416,7 +10585,7 @@
       <c r="E365" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F365" s="8" t="s">
+      <c r="F365" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10436,7 +10605,7 @@
       <c r="E366" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F366" s="8" t="s">
+      <c r="F366" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10456,7 +10625,7 @@
       <c r="E367" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F367" s="8" t="s">
+      <c r="F367" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10476,7 +10645,7 @@
       <c r="E368" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F368" s="8" t="s">
+      <c r="F368" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10496,7 +10665,7 @@
       <c r="E369" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F369" s="8" t="s">
+      <c r="F369" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10516,7 +10685,7 @@
       <c r="E370" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F370" s="8" t="s">
+      <c r="F370" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10536,7 +10705,7 @@
       <c r="E371" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F371" s="8" t="s">
+      <c r="F371" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10556,7 +10725,7 @@
       <c r="E372" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F372" s="8" t="s">
+      <c r="F372" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10576,7 +10745,7 @@
       <c r="E373" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F373" s="8" t="s">
+      <c r="F373" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10596,7 +10765,7 @@
       <c r="E374" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F374" s="8" t="s">
+      <c r="F374" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10616,7 +10785,7 @@
       <c r="E375" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F375" s="8" t="s">
+      <c r="F375" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10636,7 +10805,7 @@
       <c r="E376" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F376" s="8" t="s">
+      <c r="F376" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10656,7 +10825,7 @@
       <c r="E377" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F377" s="8" t="s">
+      <c r="F377" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10676,7 +10845,7 @@
       <c r="E378" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F378" s="8" t="s">
+      <c r="F378" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10696,7 +10865,7 @@
       <c r="E379" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F379" s="8" t="s">
+      <c r="F379" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10716,7 +10885,7 @@
       <c r="E380" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F380" s="8" t="s">
+      <c r="F380" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10736,7 +10905,7 @@
       <c r="E381" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F381" s="8" t="s">
+      <c r="F381" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10756,7 +10925,7 @@
       <c r="E382" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F382" s="8" t="s">
+      <c r="F382" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10776,7 +10945,7 @@
       <c r="E383" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F383" s="8" t="s">
+      <c r="F383" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10796,7 +10965,7 @@
       <c r="E384" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F384" s="8" t="s">
+      <c r="F384" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10816,7 +10985,7 @@
       <c r="E385" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F385" s="8" t="s">
+      <c r="F385" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10836,7 +11005,7 @@
       <c r="E386" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F386" s="8" t="s">
+      <c r="F386" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10856,7 +11025,7 @@
       <c r="E387" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F387" s="8" t="s">
+      <c r="F387" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10876,7 +11045,7 @@
       <c r="E388" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F388" s="8" t="s">
+      <c r="F388" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10896,7 +11065,7 @@
       <c r="E389" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="F389" s="8" t="s">
+      <c r="F389" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -10930,7 +11099,7 @@
       <c r="E391" s="5" t="s">
         <v>936</v>
       </c>
-      <c r="F391" s="8" t="s">
+      <c r="F391" s="5" t="s">
         <v>775</v>
       </c>
     </row>
@@ -10992,7 +11161,7 @@
       <c r="E395" s="5" t="s">
         <v>726</v>
       </c>
-      <c r="F395" s="8" t="s">
+      <c r="F395" s="5" t="s">
         <v>727</v>
       </c>
     </row>
@@ -11012,7 +11181,7 @@
       <c r="E396" s="5" t="s">
         <v>726</v>
       </c>
-      <c r="F396" s="8" t="s">
+      <c r="F396" s="5" t="s">
         <v>727</v>
       </c>
     </row>
@@ -11032,7 +11201,7 @@
       <c r="E397" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F397" s="8" t="s">
+      <c r="F397" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -11066,7 +11235,7 @@
       <c r="E399" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F399" s="8" t="s">
+      <c r="F399" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11086,7 +11255,7 @@
       <c r="E400" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="F400" s="8" t="s">
+      <c r="F400" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11106,7 +11275,7 @@
       <c r="E401" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F401" s="8" t="s">
+      <c r="F401" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11126,7 +11295,7 @@
       <c r="E402" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F402" s="8" t="s">
+      <c r="F402" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11146,7 +11315,7 @@
       <c r="E403" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="F403" s="8" t="s">
+      <c r="F403" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11166,7 +11335,7 @@
       <c r="E404" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="F404" s="8" t="s">
+      <c r="F404" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11186,7 +11355,7 @@
       <c r="E405" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F405" s="8" t="s">
+      <c r="F405" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11206,7 +11375,7 @@
       <c r="E406" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="F406" s="8" t="s">
+      <c r="F406" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11226,7 +11395,7 @@
       <c r="E407" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F407" s="8" t="s">
+      <c r="F407" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11246,7 +11415,7 @@
       <c r="E408" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F408" s="8" t="s">
+      <c r="F408" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11266,7 +11435,7 @@
       <c r="E409" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="F409" s="8" t="s">
+      <c r="F409" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11286,7 +11455,7 @@
       <c r="E410" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="F410" s="8" t="s">
+      <c r="F410" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11306,7 +11475,7 @@
       <c r="E411" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F411" s="8" t="s">
+      <c r="F411" s="5" t="s">
         <v>729</v>
       </c>
     </row>
@@ -11326,7 +11495,7 @@
       <c r="E412" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F412" s="8" t="s">
+      <c r="F412" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11346,7 +11515,7 @@
       <c r="E413" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F413" s="8" t="s">
+      <c r="F413" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11366,7 +11535,7 @@
       <c r="E414" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F414" s="8" t="s">
+      <c r="F414" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11386,7 +11555,7 @@
       <c r="E415" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F415" s="8" t="s">
+      <c r="F415" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11406,7 +11575,7 @@
       <c r="E416" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F416" s="8" t="s">
+      <c r="F416" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11426,7 +11595,7 @@
       <c r="E417" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="F417" s="8" t="s">
+      <c r="F417" s="5" t="s">
         <v>966</v>
       </c>
     </row>
@@ -11446,7 +11615,497 @@
       <c r="E418" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="F418" s="8" t="s">
+      <c r="F418" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>983</v>
+      </c>
+      <c r="B419" t="s">
+        <v>984</v>
+      </c>
+      <c r="C419" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D419" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E419" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F419" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>983</v>
+      </c>
+      <c r="B420" t="s">
+        <v>985</v>
+      </c>
+      <c r="C420" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D420" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E420" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F420" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>983</v>
+      </c>
+      <c r="B421" t="s">
+        <v>986</v>
+      </c>
+      <c r="C421" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D421" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E421" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F421" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>983</v>
+      </c>
+      <c r="B422" t="s">
+        <v>987</v>
+      </c>
+      <c r="C422" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D422" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E422" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F422" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>983</v>
+      </c>
+      <c r="B423" t="s">
+        <v>988</v>
+      </c>
+      <c r="C423" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D423" s="3" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>983</v>
+      </c>
+      <c r="B424" t="s">
+        <v>989</v>
+      </c>
+      <c r="C424" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D424" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F424" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>983</v>
+      </c>
+      <c r="B425" t="s">
+        <v>990</v>
+      </c>
+      <c r="C425" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D425" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E425" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F425" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>983</v>
+      </c>
+      <c r="B426" t="s">
+        <v>991</v>
+      </c>
+      <c r="C426" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D426" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E426" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F426" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>983</v>
+      </c>
+      <c r="B427" t="s">
+        <v>992</v>
+      </c>
+      <c r="C427" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D427" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E427" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F427" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>983</v>
+      </c>
+      <c r="B428" t="s">
+        <v>993</v>
+      </c>
+      <c r="C428" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D428" s="3" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>983</v>
+      </c>
+      <c r="B429" t="s">
+        <v>994</v>
+      </c>
+      <c r="C429" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D429" s="3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E429" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F429" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>983</v>
+      </c>
+      <c r="B430" t="s">
+        <v>995</v>
+      </c>
+      <c r="C430" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D430" s="3" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>983</v>
+      </c>
+      <c r="B431" t="s">
+        <v>996</v>
+      </c>
+      <c r="C431" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D431" s="3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E431" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F431" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>983</v>
+      </c>
+      <c r="B432" t="s">
+        <v>997</v>
+      </c>
+      <c r="C432" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D432" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E432" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F432" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>983</v>
+      </c>
+      <c r="B433" t="s">
+        <v>998</v>
+      </c>
+      <c r="C433" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D433" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E433" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F433" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>983</v>
+      </c>
+      <c r="B434" t="s">
+        <v>999</v>
+      </c>
+      <c r="C434" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D434" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E434" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="F434" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B435" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C435" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D435" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E435" s="5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F435" s="5" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B436" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C436" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D436" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E436" s="5" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F436" s="5" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B437" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C437" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D437" s="3" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A438" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B438" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C438" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D438" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E438" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="F438" s="5" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A439" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B439" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C439" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D439" s="3" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A440" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B440" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C440" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D440" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="E440" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F440" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A441" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B441" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C441" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D441" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E441" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F441" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A442" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B442" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C442" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D442" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E442" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F442" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A443" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B443" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C443" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D443" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E443" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F443" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A444" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B444" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C444" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D444" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E444" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="F444" s="5" t="s">
         <v>729</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added validation to check that all expected surveys are in the lookup
</commit_message>
<xml_diff>
--- a/data/fff-question-lookup.xlsx
+++ b/data/fff-question-lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/FFF-RedCap/FFF-RedCap-data-processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1934" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{958E97CD-2D6D-4629-B979-F25F5EAFA873}"/>
+  <xr:revisionPtr revIDLastSave="1936" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55C2912A-2115-4BF3-A885-D54FEF52542E}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1410" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4206,8 +4206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F584"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A338" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A352" sqref="A352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10953,24 +10953,24 @@
         <v>729</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B352" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C352" s="10" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
       <c r="D352" s="3" t="s">
-        <v>423</v>
+        <v>490</v>
       </c>
       <c r="E352" s="5" t="s">
-        <v>728</v>
+        <v>756</v>
       </c>
       <c r="F352" s="5" t="s">
-        <v>729</v>
+        <v>757</v>
       </c>
     </row>
     <row r="353" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -10978,13 +10978,13 @@
         <v>386</v>
       </c>
       <c r="B353" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C353" s="10" t="s">
         <v>412</v>
       </c>
       <c r="D353" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E353" s="5" t="s">
         <v>756</v>
@@ -10998,13 +10998,13 @@
         <v>386</v>
       </c>
       <c r="B354" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C354" s="10" t="s">
         <v>412</v>
       </c>
       <c r="D354" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E354" s="5" t="s">
         <v>756</v>
@@ -11018,13 +11018,13 @@
         <v>386</v>
       </c>
       <c r="B355" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C355" s="10" t="s">
         <v>412</v>
       </c>
       <c r="D355" s="3" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="E355" s="5" t="s">
         <v>756</v>
@@ -11038,13 +11038,13 @@
         <v>386</v>
       </c>
       <c r="B356" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C356" s="10" t="s">
         <v>412</v>
       </c>
       <c r="D356" s="3" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E356" s="5" t="s">
         <v>756</v>
@@ -11058,13 +11058,13 @@
         <v>386</v>
       </c>
       <c r="B357" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C357" s="10" t="s">
         <v>412</v>
       </c>
       <c r="D357" s="3" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="E357" s="5" t="s">
         <v>756</v>
@@ -11078,13 +11078,13 @@
         <v>386</v>
       </c>
       <c r="B358" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C358" s="10" t="s">
         <v>412</v>
       </c>
       <c r="D358" s="3" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E358" s="5" t="s">
         <v>756</v>
@@ -11093,44 +11093,44 @@
         <v>757</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>386</v>
       </c>
       <c r="B359" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C359" s="10" t="s">
-        <v>412</v>
+        <v>389</v>
       </c>
       <c r="D359" s="3" t="s">
-        <v>500</v>
+        <v>423</v>
       </c>
       <c r="E359" s="5" t="s">
-        <v>756</v>
+        <v>728</v>
       </c>
       <c r="F359" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>850</v>
+      </c>
+      <c r="B360" t="s">
+        <v>851</v>
+      </c>
+      <c r="C360" s="10" t="s">
+        <v>896</v>
+      </c>
+      <c r="D360" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="E360" s="5" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F360" s="5" t="s">
         <v>757</v>
-      </c>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A360" t="s">
-        <v>386</v>
-      </c>
-      <c r="B360" t="s">
-        <v>358</v>
-      </c>
-      <c r="C360" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="D360" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="E360" s="5" t="s">
-        <v>728</v>
-      </c>
-      <c r="F360" s="5" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="361" spans="1:6" ht="360" x14ac:dyDescent="0.3">
@@ -11138,13 +11138,13 @@
         <v>850</v>
       </c>
       <c r="B361" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C361" s="10" t="s">
         <v>896</v>
       </c>
       <c r="D361" s="3" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E361" s="5" t="s">
         <v>1249</v>
@@ -11158,13 +11158,13 @@
         <v>850</v>
       </c>
       <c r="B362" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C362" s="10" t="s">
         <v>896</v>
       </c>
       <c r="D362" s="3" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="E362" s="5" t="s">
         <v>1249</v>
@@ -11178,13 +11178,13 @@
         <v>850</v>
       </c>
       <c r="B363" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C363" s="10" t="s">
         <v>896</v>
       </c>
       <c r="D363" s="3" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E363" s="5" t="s">
         <v>1249</v>
@@ -11193,18 +11193,18 @@
         <v>757</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>850</v>
       </c>
       <c r="B364" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C364" s="10" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D364" s="3" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="E364" s="5" t="s">
         <v>1249</v>
@@ -11218,13 +11218,13 @@
         <v>850</v>
       </c>
       <c r="B365" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C365" s="10" t="s">
         <v>895</v>
       </c>
       <c r="D365" s="3" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E365" s="5" t="s">
         <v>1249</v>
@@ -11238,13 +11238,13 @@
         <v>850</v>
       </c>
       <c r="B366" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C366" s="10" t="s">
         <v>895</v>
       </c>
       <c r="D366" s="3" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="E366" s="5" t="s">
         <v>1249</v>
@@ -11258,13 +11258,13 @@
         <v>850</v>
       </c>
       <c r="B367" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C367" s="10" t="s">
         <v>895</v>
       </c>
       <c r="D367" s="3" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="E367" s="5" t="s">
         <v>1249</v>
@@ -11273,21 +11273,21 @@
         <v>757</v>
       </c>
     </row>
-    <row r="368" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>850</v>
       </c>
       <c r="B368" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C368" s="10" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D368" s="3" t="s">
-        <v>904</v>
+        <v>913</v>
       </c>
       <c r="E368" s="5" t="s">
-        <v>1249</v>
+        <v>934</v>
       </c>
       <c r="F368" s="5" t="s">
         <v>757</v>
@@ -11298,13 +11298,13 @@
         <v>850</v>
       </c>
       <c r="B369" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C369" s="10" t="s">
         <v>894</v>
       </c>
       <c r="D369" s="3" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="E369" s="5" t="s">
         <v>934</v>
@@ -11318,13 +11318,13 @@
         <v>850</v>
       </c>
       <c r="B370" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C370" s="10" t="s">
         <v>894</v>
       </c>
       <c r="D370" s="3" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="E370" s="5" t="s">
         <v>934</v>
@@ -11338,13 +11338,13 @@
         <v>850</v>
       </c>
       <c r="B371" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C371" s="10" t="s">
         <v>894</v>
       </c>
       <c r="D371" s="3" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="E371" s="5" t="s">
         <v>934</v>
@@ -11358,13 +11358,13 @@
         <v>850</v>
       </c>
       <c r="B372" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C372" s="10" t="s">
         <v>894</v>
       </c>
       <c r="D372" s="3" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="E372" s="5" t="s">
         <v>934</v>
@@ -11373,18 +11373,18 @@
         <v>757</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>850</v>
       </c>
       <c r="B373" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C373" s="10" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D373" s="3" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="E373" s="5" t="s">
         <v>934</v>
@@ -11398,13 +11398,13 @@
         <v>850</v>
       </c>
       <c r="B374" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C374" s="10" t="s">
         <v>893</v>
       </c>
       <c r="D374" s="3" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="E374" s="5" t="s">
         <v>934</v>
@@ -11418,13 +11418,13 @@
         <v>850</v>
       </c>
       <c r="B375" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C375" s="10" t="s">
         <v>893</v>
       </c>
       <c r="D375" s="3" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="E375" s="5" t="s">
         <v>934</v>
@@ -11438,13 +11438,13 @@
         <v>850</v>
       </c>
       <c r="B376" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C376" s="10" t="s">
         <v>893</v>
       </c>
       <c r="D376" s="3" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="E376" s="5" t="s">
         <v>934</v>
@@ -11453,18 +11453,18 @@
         <v>757</v>
       </c>
     </row>
-    <row r="377" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>850</v>
       </c>
       <c r="B377" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C377" s="10" t="s">
         <v>893</v>
       </c>
       <c r="D377" s="3" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="E377" s="5" t="s">
         <v>934</v>
@@ -11473,18 +11473,18 @@
         <v>757</v>
       </c>
     </row>
-    <row r="378" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>850</v>
       </c>
       <c r="B378" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C378" s="10" t="s">
         <v>893</v>
       </c>
       <c r="D378" s="3" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="E378" s="5" t="s">
         <v>934</v>
@@ -11498,13 +11498,13 @@
         <v>850</v>
       </c>
       <c r="B379" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C379" s="10" t="s">
         <v>893</v>
       </c>
       <c r="D379" s="3" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="E379" s="5" t="s">
         <v>934</v>
@@ -11513,18 +11513,18 @@
         <v>757</v>
       </c>
     </row>
-    <row r="380" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>850</v>
       </c>
       <c r="B380" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C380" s="10" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D380" s="3" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="E380" s="5" t="s">
         <v>934</v>
@@ -11538,13 +11538,13 @@
         <v>850</v>
       </c>
       <c r="B381" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C381" s="10" t="s">
         <v>892</v>
       </c>
       <c r="D381" s="3" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E381" s="5" t="s">
         <v>934</v>
@@ -11558,13 +11558,13 @@
         <v>850</v>
       </c>
       <c r="B382" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C382" s="10" t="s">
         <v>892</v>
       </c>
       <c r="D382" s="3" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="E382" s="5" t="s">
         <v>934</v>
@@ -11578,13 +11578,13 @@
         <v>850</v>
       </c>
       <c r="B383" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C383" s="10" t="s">
         <v>892</v>
       </c>
       <c r="D383" s="3" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="E383" s="5" t="s">
         <v>934</v>
@@ -11598,13 +11598,13 @@
         <v>850</v>
       </c>
       <c r="B384" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C384" s="10" t="s">
         <v>892</v>
       </c>
       <c r="D384" s="3" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="E384" s="5" t="s">
         <v>934</v>
@@ -11613,18 +11613,18 @@
         <v>757</v>
       </c>
     </row>
-    <row r="385" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>850</v>
       </c>
       <c r="B385" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C385" s="10" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="D385" s="3" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="E385" s="5" t="s">
         <v>934</v>
@@ -11638,13 +11638,13 @@
         <v>850</v>
       </c>
       <c r="B386" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="C386" s="10" t="s">
         <v>890</v>
       </c>
       <c r="D386" s="3" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="E386" s="5" t="s">
         <v>934</v>
@@ -11658,13 +11658,13 @@
         <v>850</v>
       </c>
       <c r="B387" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C387" s="10" t="s">
         <v>890</v>
       </c>
       <c r="D387" s="3" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="E387" s="5" t="s">
         <v>934</v>
@@ -11678,13 +11678,13 @@
         <v>850</v>
       </c>
       <c r="B388" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C388" s="10" t="s">
         <v>890</v>
       </c>
       <c r="D388" s="3" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="E388" s="5" t="s">
         <v>934</v>
@@ -11698,33 +11698,33 @@
         <v>850</v>
       </c>
       <c r="B389" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C389" s="10" t="s">
         <v>890</v>
       </c>
       <c r="D389" s="3" t="s">
-        <v>925</v>
-      </c>
-      <c r="E389" s="5" t="s">
-        <v>934</v>
-      </c>
-      <c r="F389" s="5" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="390" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>850</v>
       </c>
       <c r="B390" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C390" s="10" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D390" s="3" t="s">
-        <v>926</v>
+        <v>927</v>
+      </c>
+      <c r="E390" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="F390" s="5" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="391" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -11732,19 +11732,13 @@
         <v>850</v>
       </c>
       <c r="B391" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C391" s="10" t="s">
         <v>889</v>
       </c>
       <c r="D391" s="3" t="s">
-        <v>927</v>
-      </c>
-      <c r="E391" s="5" t="s">
-        <v>935</v>
-      </c>
-      <c r="F391" s="5" t="s">
-        <v>775</v>
+        <v>928</v>
       </c>
     </row>
     <row r="392" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -11752,13 +11746,13 @@
         <v>850</v>
       </c>
       <c r="B392" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C392" s="10" t="s">
         <v>889</v>
       </c>
       <c r="D392" s="3" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
     </row>
     <row r="393" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -11766,13 +11760,13 @@
         <v>850</v>
       </c>
       <c r="B393" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C393" s="10" t="s">
         <v>889</v>
       </c>
       <c r="D393" s="3" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
     </row>
     <row r="394" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -11780,13 +11774,19 @@
         <v>850</v>
       </c>
       <c r="B394" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C394" s="10" t="s">
         <v>889</v>
       </c>
       <c r="D394" s="3" t="s">
-        <v>930</v>
+        <v>931</v>
+      </c>
+      <c r="E394" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F394" s="5" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="395" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -11794,13 +11794,13 @@
         <v>850</v>
       </c>
       <c r="B395" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C395" s="10" t="s">
         <v>889</v>
       </c>
       <c r="D395" s="3" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="E395" s="5" t="s">
         <v>726</v>
@@ -11809,95 +11809,95 @@
         <v>727</v>
       </c>
     </row>
-    <row r="396" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>850</v>
       </c>
       <c r="B396" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C396" s="10" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="D396" s="3" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E396" s="5" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="F396" s="5" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="397" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>850</v>
       </c>
       <c r="B397" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C397" s="10" t="s">
-        <v>891</v>
+        <v>389</v>
       </c>
       <c r="D397" s="3" t="s">
-        <v>933</v>
-      </c>
-      <c r="E397" s="5" t="s">
-        <v>728</v>
-      </c>
-      <c r="F397" s="5" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>850</v>
+        <v>936</v>
       </c>
       <c r="B398" t="s">
-        <v>888</v>
+        <v>937</v>
       </c>
       <c r="C398" s="10" t="s">
-        <v>389</v>
+        <v>950</v>
       </c>
       <c r="D398" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="399" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>952</v>
+      </c>
+      <c r="E398" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="F398" s="5" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>936</v>
       </c>
       <c r="B399" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C399" s="10" t="s">
         <v>950</v>
       </c>
       <c r="D399" s="3" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="E399" s="5" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="F399" s="5" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="400" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>936</v>
       </c>
       <c r="B400" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C400" s="10" t="s">
         <v>950</v>
       </c>
       <c r="D400" s="3" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="E400" s="5" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="F400" s="5" t="s">
         <v>965</v>
@@ -11908,13 +11908,13 @@
         <v>936</v>
       </c>
       <c r="B401" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C401" s="10" t="s">
         <v>950</v>
       </c>
       <c r="D401" s="3" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="E401" s="5" t="s">
         <v>964</v>
@@ -11928,16 +11928,16 @@
         <v>936</v>
       </c>
       <c r="B402" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C402" s="10" t="s">
         <v>950</v>
       </c>
       <c r="D402" s="3" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="E402" s="5" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="F402" s="5" t="s">
         <v>965</v>
@@ -11948,13 +11948,13 @@
         <v>936</v>
       </c>
       <c r="B403" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="C403" s="10" t="s">
         <v>950</v>
       </c>
       <c r="D403" s="3" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="E403" s="5" t="s">
         <v>967</v>
@@ -11968,56 +11968,56 @@
         <v>936</v>
       </c>
       <c r="B404" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C404" s="10" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="D404" s="3" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="E404" s="5" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F404" s="5" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="405" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>936</v>
       </c>
       <c r="B405" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C405" s="10" t="s">
         <v>951</v>
       </c>
       <c r="D405" s="3" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="E405" s="5" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="F405" s="5" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="406" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>936</v>
       </c>
       <c r="B406" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C406" s="10" t="s">
         <v>951</v>
       </c>
       <c r="D406" s="3" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="E406" s="5" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="F406" s="5" t="s">
         <v>965</v>
@@ -12028,13 +12028,13 @@
         <v>936</v>
       </c>
       <c r="B407" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="C407" s="10" t="s">
         <v>951</v>
       </c>
       <c r="D407" s="3" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E407" s="5" t="s">
         <v>964</v>
@@ -12048,16 +12048,16 @@
         <v>936</v>
       </c>
       <c r="B408" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C408" s="10" t="s">
         <v>951</v>
       </c>
       <c r="D408" s="3" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="E408" s="5" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="F408" s="5" t="s">
         <v>965</v>
@@ -12068,13 +12068,13 @@
         <v>936</v>
       </c>
       <c r="B409" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C409" s="10" t="s">
         <v>951</v>
       </c>
       <c r="D409" s="3" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="E409" s="5" t="s">
         <v>967</v>
@@ -12083,44 +12083,44 @@
         <v>965</v>
       </c>
     </row>
-    <row r="410" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>936</v>
       </c>
       <c r="B410" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C410" s="10" t="s">
-        <v>951</v>
+        <v>389</v>
       </c>
       <c r="D410" s="3" t="s">
-        <v>963</v>
+        <v>423</v>
       </c>
       <c r="E410" s="5" t="s">
-        <v>967</v>
+        <v>728</v>
       </c>
       <c r="F410" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>968</v>
+      </c>
+      <c r="B411" t="s">
+        <v>969</v>
+      </c>
+      <c r="C411" s="10" t="s">
+        <v>975</v>
+      </c>
+      <c r="D411" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="E411" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="F411" s="5" t="s">
         <v>965</v>
-      </c>
-    </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A411" t="s">
-        <v>936</v>
-      </c>
-      <c r="B411" t="s">
-        <v>949</v>
-      </c>
-      <c r="C411" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="D411" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="E411" s="5" t="s">
-        <v>728</v>
-      </c>
-      <c r="F411" s="5" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="412" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -12128,13 +12128,13 @@
         <v>968</v>
       </c>
       <c r="B412" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C412" s="10" t="s">
         <v>975</v>
       </c>
       <c r="D412" s="3" t="s">
-        <v>952</v>
+        <v>976</v>
       </c>
       <c r="E412" s="5" t="s">
         <v>964</v>
@@ -12148,13 +12148,13 @@
         <v>968</v>
       </c>
       <c r="B413" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C413" s="10" t="s">
         <v>975</v>
       </c>
       <c r="D413" s="3" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="E413" s="5" t="s">
         <v>964</v>
@@ -12168,13 +12168,13 @@
         <v>968</v>
       </c>
       <c r="B414" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C414" s="10" t="s">
-        <v>975</v>
+        <v>951</v>
       </c>
       <c r="D414" s="3" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="E414" s="5" t="s">
         <v>964</v>
@@ -12188,13 +12188,13 @@
         <v>968</v>
       </c>
       <c r="B415" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="C415" s="10" t="s">
         <v>951</v>
       </c>
       <c r="D415" s="3" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="E415" s="5" t="s">
         <v>964</v>
@@ -12208,13 +12208,13 @@
         <v>968</v>
       </c>
       <c r="B416" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C416" s="10" t="s">
         <v>951</v>
       </c>
       <c r="D416" s="3" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="E416" s="5" t="s">
         <v>964</v>
@@ -12223,44 +12223,44 @@
         <v>965</v>
       </c>
     </row>
-    <row r="417" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>968</v>
       </c>
       <c r="B417" t="s">
-        <v>974</v>
+        <v>981</v>
       </c>
       <c r="C417" s="10" t="s">
-        <v>951</v>
+        <v>389</v>
       </c>
       <c r="D417" s="3" t="s">
-        <v>980</v>
+        <v>423</v>
       </c>
       <c r="E417" s="5" t="s">
-        <v>964</v>
+        <v>728</v>
       </c>
       <c r="F417" s="5" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.3">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
-        <v>968</v>
+        <v>982</v>
       </c>
       <c r="B418" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="C418" s="10" t="s">
-        <v>389</v>
+        <v>999</v>
       </c>
       <c r="D418" s="3" t="s">
-        <v>423</v>
+        <v>1002</v>
       </c>
       <c r="E418" s="5" t="s">
-        <v>728</v>
+        <v>1008</v>
       </c>
       <c r="F418" s="5" t="s">
-        <v>729</v>
+        <v>757</v>
       </c>
     </row>
     <row r="419" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12268,13 +12268,13 @@
         <v>982</v>
       </c>
       <c r="B419" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C419" s="10" t="s">
         <v>999</v>
       </c>
       <c r="D419" s="3" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="E419" s="5" t="s">
         <v>1008</v>
@@ -12288,13 +12288,13 @@
         <v>982</v>
       </c>
       <c r="B420" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C420" s="10" t="s">
         <v>999</v>
       </c>
       <c r="D420" s="3" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="E420" s="5" t="s">
         <v>1008</v>
@@ -12308,19 +12308,19 @@
         <v>982</v>
       </c>
       <c r="B421" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C421" s="10" t="s">
         <v>999</v>
       </c>
       <c r="D421" s="3" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E421" s="5" t="s">
-        <v>1008</v>
+        <v>726</v>
       </c>
       <c r="F421" s="5" t="s">
-        <v>757</v>
+        <v>727</v>
       </c>
     </row>
     <row r="422" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12328,19 +12328,13 @@
         <v>982</v>
       </c>
       <c r="B422" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="C422" s="10" t="s">
         <v>999</v>
       </c>
       <c r="D422" s="3" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E422" s="5" t="s">
-        <v>726</v>
-      </c>
-      <c r="F422" s="5" t="s">
-        <v>727</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="423" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12348,13 +12342,19 @@
         <v>982</v>
       </c>
       <c r="B423" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C423" s="10" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D423" s="3" t="s">
-        <v>1007</v>
+        <v>1002</v>
+      </c>
+      <c r="E423" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F423" s="5" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="424" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12362,13 +12362,13 @@
         <v>982</v>
       </c>
       <c r="B424" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="C424" s="10" t="s">
         <v>1000</v>
       </c>
       <c r="D424" s="3" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="E424" s="5" t="s">
         <v>1008</v>
@@ -12382,13 +12382,13 @@
         <v>982</v>
       </c>
       <c r="B425" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C425" s="10" t="s">
         <v>1000</v>
       </c>
       <c r="D425" s="3" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="E425" s="5" t="s">
         <v>1008</v>
@@ -12402,19 +12402,19 @@
         <v>982</v>
       </c>
       <c r="B426" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C426" s="10" t="s">
         <v>1000</v>
       </c>
       <c r="D426" s="3" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="E426" s="5" t="s">
-        <v>1008</v>
+        <v>726</v>
       </c>
       <c r="F426" s="5" t="s">
-        <v>757</v>
+        <v>727</v>
       </c>
     </row>
     <row r="427" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12422,19 +12422,13 @@
         <v>982</v>
       </c>
       <c r="B427" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C427" s="10" t="s">
         <v>1000</v>
       </c>
       <c r="D427" s="3" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E427" s="5" t="s">
-        <v>726</v>
-      </c>
-      <c r="F427" s="5" t="s">
-        <v>727</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="428" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12442,13 +12436,19 @@
         <v>982</v>
       </c>
       <c r="B428" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C428" s="10" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="D428" s="3" t="s">
-        <v>1007</v>
+        <v>1010</v>
+      </c>
+      <c r="E428" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F428" s="5" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="429" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12456,19 +12456,13 @@
         <v>982</v>
       </c>
       <c r="B429" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="C429" s="10" t="s">
         <v>1001</v>
       </c>
       <c r="D429" s="3" t="s">
-        <v>1010</v>
-      </c>
-      <c r="E429" s="5" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F429" s="5" t="s">
-        <v>757</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="430" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12476,13 +12470,19 @@
         <v>982</v>
       </c>
       <c r="B430" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C430" s="10" t="s">
         <v>1001</v>
       </c>
       <c r="D430" s="3" t="s">
-        <v>1006</v>
+        <v>1013</v>
+      </c>
+      <c r="E430" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F430" s="5" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="431" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -12490,13 +12490,13 @@
         <v>982</v>
       </c>
       <c r="B431" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="C431" s="10" t="s">
         <v>1001</v>
       </c>
       <c r="D431" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E431" s="5" t="s">
         <v>1008</v>
@@ -12510,99 +12510,99 @@
         <v>982</v>
       </c>
       <c r="B432" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C432" s="10" t="s">
         <v>1001</v>
       </c>
       <c r="D432" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E432" s="5" t="s">
-        <v>1008</v>
+        <v>726</v>
       </c>
       <c r="F432" s="5" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="433" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>982</v>
       </c>
       <c r="B433" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C433" s="10" t="s">
-        <v>1001</v>
+        <v>389</v>
       </c>
       <c r="D433" s="3" t="s">
-        <v>1011</v>
+        <v>423</v>
       </c>
       <c r="E433" s="5" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="F433" s="5" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.3">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
-        <v>982</v>
+        <v>1014</v>
       </c>
       <c r="B434" t="s">
-        <v>998</v>
+        <v>1015</v>
       </c>
       <c r="C434" s="10" t="s">
-        <v>389</v>
+        <v>1030</v>
       </c>
       <c r="D434" s="3" t="s">
-        <v>423</v>
+        <v>1024</v>
       </c>
       <c r="E434" s="5" t="s">
-        <v>728</v>
+        <v>1031</v>
       </c>
       <c r="F434" s="5" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="435" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>1014</v>
       </c>
       <c r="B435" t="s">
-        <v>1015</v>
+        <v>1069</v>
       </c>
       <c r="C435" s="10" t="s">
-        <v>1030</v>
+        <v>1025</v>
       </c>
       <c r="D435" s="3" t="s">
-        <v>1024</v>
+        <v>517</v>
       </c>
       <c r="E435" s="5" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="F435" s="5" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="436" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>1014</v>
       </c>
       <c r="B436" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="C436" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D436" s="3" t="s">
-        <v>517</v>
+        <v>1092</v>
       </c>
       <c r="E436" s="5" t="s">
-        <v>1032</v>
+        <v>821</v>
       </c>
       <c r="F436" s="5" t="s">
-        <v>1033</v>
+        <v>822</v>
       </c>
     </row>
     <row r="437" spans="1:6" x14ac:dyDescent="0.3">
@@ -12610,13 +12610,13 @@
         <v>1014</v>
       </c>
       <c r="B437" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="C437" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D437" s="3" t="s">
-        <v>1092</v>
+        <v>519</v>
       </c>
       <c r="E437" s="5" t="s">
         <v>821</v>
@@ -12630,13 +12630,13 @@
         <v>1014</v>
       </c>
       <c r="B438" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="C438" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D438" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E438" s="5" t="s">
         <v>821</v>
@@ -12650,13 +12650,13 @@
         <v>1014</v>
       </c>
       <c r="B439" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C439" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D439" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E439" s="5" t="s">
         <v>821</v>
@@ -12670,13 +12670,13 @@
         <v>1014</v>
       </c>
       <c r="B440" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="C440" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D440" s="3" t="s">
-        <v>521</v>
+        <v>841</v>
       </c>
       <c r="E440" s="5" t="s">
         <v>821</v>
@@ -12690,13 +12690,13 @@
         <v>1014</v>
       </c>
       <c r="B441" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C441" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D441" s="3" t="s">
-        <v>841</v>
+        <v>522</v>
       </c>
       <c r="E441" s="5" t="s">
         <v>821</v>
@@ -12710,13 +12710,13 @@
         <v>1014</v>
       </c>
       <c r="B442" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C442" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D442" s="3" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="E442" s="5" t="s">
         <v>821</v>
@@ -12730,13 +12730,13 @@
         <v>1014</v>
       </c>
       <c r="B443" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C443" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D443" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E443" s="5" t="s">
         <v>821</v>
@@ -12750,13 +12750,13 @@
         <v>1014</v>
       </c>
       <c r="B444" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="C444" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D444" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E444" s="5" t="s">
         <v>821</v>
@@ -12770,13 +12770,13 @@
         <v>1014</v>
       </c>
       <c r="B445" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C445" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D445" s="3" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="E445" s="5" t="s">
         <v>821</v>
@@ -12790,13 +12790,13 @@
         <v>1014</v>
       </c>
       <c r="B446" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C446" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D446" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E446" s="5" t="s">
         <v>821</v>
@@ -12810,13 +12810,13 @@
         <v>1014</v>
       </c>
       <c r="B447" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C447" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D447" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E447" s="5" t="s">
         <v>821</v>
@@ -12830,13 +12830,13 @@
         <v>1014</v>
       </c>
       <c r="B448" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C448" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D448" s="3" t="s">
-        <v>528</v>
+        <v>1094</v>
       </c>
       <c r="E448" s="5" t="s">
         <v>821</v>
@@ -12850,13 +12850,13 @@
         <v>1014</v>
       </c>
       <c r="B449" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C449" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D449" s="3" t="s">
-        <v>1094</v>
+        <v>530</v>
       </c>
       <c r="E449" s="5" t="s">
         <v>821</v>
@@ -12870,13 +12870,13 @@
         <v>1014</v>
       </c>
       <c r="B450" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C450" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D450" s="3" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E450" s="5" t="s">
         <v>821</v>
@@ -12890,13 +12890,13 @@
         <v>1014</v>
       </c>
       <c r="B451" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C451" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D451" s="3" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E451" s="5" t="s">
         <v>821</v>
@@ -12910,13 +12910,13 @@
         <v>1014</v>
       </c>
       <c r="B452" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C452" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D452" s="3" t="s">
-        <v>532</v>
+        <v>1095</v>
       </c>
       <c r="E452" s="5" t="s">
         <v>821</v>
@@ -12930,13 +12930,13 @@
         <v>1014</v>
       </c>
       <c r="B453" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C453" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D453" s="3" t="s">
-        <v>1095</v>
+        <v>534</v>
       </c>
       <c r="E453" s="5" t="s">
         <v>821</v>
@@ -12950,13 +12950,13 @@
         <v>1014</v>
       </c>
       <c r="B454" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="C454" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D454" s="3" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E454" s="5" t="s">
         <v>821</v>
@@ -12970,13 +12970,13 @@
         <v>1014</v>
       </c>
       <c r="B455" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C455" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D455" s="3" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E455" s="5" t="s">
         <v>821</v>
@@ -12990,13 +12990,13 @@
         <v>1014</v>
       </c>
       <c r="B456" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="C456" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D456" s="3" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E456" s="5" t="s">
         <v>821</v>
@@ -13010,13 +13010,13 @@
         <v>1014</v>
       </c>
       <c r="B457" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C457" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D457" s="3" t="s">
-        <v>537</v>
+        <v>456</v>
       </c>
       <c r="E457" s="5" t="s">
         <v>821</v>
@@ -13030,13 +13030,13 @@
         <v>1014</v>
       </c>
       <c r="B458" t="s">
-        <v>1091</v>
+        <v>1016</v>
       </c>
       <c r="C458" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="D458" s="3" t="s">
-        <v>456</v>
+        <v>1093</v>
       </c>
       <c r="E458" s="5" t="s">
         <v>821</v>
@@ -13050,19 +13050,19 @@
         <v>1014</v>
       </c>
       <c r="B459" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C459" s="10" t="s">
-        <v>1025</v>
+        <v>1096</v>
       </c>
       <c r="D459" s="3" t="s">
-        <v>1093</v>
+        <v>1026</v>
       </c>
       <c r="E459" s="5" t="s">
-        <v>821</v>
+        <v>771</v>
       </c>
       <c r="F459" s="5" t="s">
-        <v>822</v>
+        <v>759</v>
       </c>
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.3">
@@ -13070,33 +13070,33 @@
         <v>1014</v>
       </c>
       <c r="B460" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C460" s="10" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D460" s="3" t="s">
-        <v>1026</v>
-      </c>
-      <c r="E460" s="5" t="s">
-        <v>771</v>
-      </c>
-      <c r="F460" s="5" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>1014</v>
       </c>
       <c r="B461" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="C461" s="10" t="s">
         <v>1097</v>
       </c>
       <c r="D461" s="3" t="s">
-        <v>1034</v>
+        <v>544</v>
+      </c>
+      <c r="E461" s="5" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F461" s="5" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="462" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -13104,13 +13104,13 @@
         <v>1014</v>
       </c>
       <c r="B462" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C462" s="10" t="s">
         <v>1097</v>
       </c>
       <c r="D462" s="3" t="s">
-        <v>544</v>
+        <v>1027</v>
       </c>
       <c r="E462" s="5" t="s">
         <v>1035</v>
@@ -13124,13 +13124,13 @@
         <v>1014</v>
       </c>
       <c r="B463" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C463" s="10" t="s">
         <v>1097</v>
       </c>
       <c r="D463" s="3" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="E463" s="5" t="s">
         <v>1035</v>
@@ -13144,13 +13144,13 @@
         <v>1014</v>
       </c>
       <c r="B464" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C464" s="10" t="s">
         <v>1097</v>
       </c>
       <c r="D464" s="3" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="E464" s="5" t="s">
         <v>1035</v>
@@ -13159,44 +13159,44 @@
         <v>757</v>
       </c>
     </row>
-    <row r="465" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>1014</v>
       </c>
       <c r="B465" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="C465" s="10" t="s">
-        <v>1097</v>
+        <v>389</v>
       </c>
       <c r="D465" s="3" t="s">
-        <v>1029</v>
+        <v>423</v>
       </c>
       <c r="E465" s="5" t="s">
-        <v>1035</v>
+        <v>728</v>
       </c>
       <c r="F465" s="5" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.3">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
-        <v>1014</v>
+        <v>1036</v>
       </c>
       <c r="B466" t="s">
-        <v>1023</v>
+        <v>1037</v>
       </c>
       <c r="C466" s="10" t="s">
-        <v>389</v>
+        <v>1125</v>
       </c>
       <c r="D466" s="3" t="s">
-        <v>423</v>
+        <v>1067</v>
       </c>
       <c r="E466" s="5" t="s">
-        <v>728</v>
+        <v>1137</v>
       </c>
       <c r="F466" s="5" t="s">
-        <v>729</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="467" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -13204,33 +13204,33 @@
         <v>1036</v>
       </c>
       <c r="B467" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C467" s="10" t="s">
         <v>1125</v>
       </c>
       <c r="D467" s="3" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E467" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F467" s="5" t="s">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="468" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>1036</v>
       </c>
       <c r="B468" t="s">
-        <v>1038</v>
+        <v>1098</v>
       </c>
       <c r="C468" s="10" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D468" s="3" t="s">
-        <v>1068</v>
+        <v>1126</v>
+      </c>
+      <c r="E468" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="F468" s="5" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="469" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -13238,13 +13238,13 @@
         <v>1036</v>
       </c>
       <c r="B469" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="C469" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D469" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="E469" s="5" t="s">
         <v>821</v>
@@ -13258,13 +13258,13 @@
         <v>1036</v>
       </c>
       <c r="B470" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C470" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D470" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="E470" s="5" t="s">
         <v>821</v>
@@ -13278,13 +13278,13 @@
         <v>1036</v>
       </c>
       <c r="B471" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C471" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D471" s="3" t="s">
-        <v>1128</v>
+        <v>527</v>
       </c>
       <c r="E471" s="5" t="s">
         <v>821</v>
@@ -13298,13 +13298,13 @@
         <v>1036</v>
       </c>
       <c r="B472" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="C472" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D472" s="3" t="s">
-        <v>527</v>
+        <v>1129</v>
       </c>
       <c r="E472" s="5" t="s">
         <v>821</v>
@@ -13318,13 +13318,13 @@
         <v>1036</v>
       </c>
       <c r="B473" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="C473" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D473" s="3" t="s">
-        <v>1129</v>
+        <v>519</v>
       </c>
       <c r="E473" s="5" t="s">
         <v>821</v>
@@ -13338,13 +13338,13 @@
         <v>1036</v>
       </c>
       <c r="B474" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C474" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D474" s="3" t="s">
-        <v>519</v>
+        <v>1130</v>
       </c>
       <c r="E474" s="5" t="s">
         <v>821</v>
@@ -13358,13 +13358,13 @@
         <v>1036</v>
       </c>
       <c r="B475" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="C475" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D475" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="E475" s="5" t="s">
         <v>821</v>
@@ -13378,13 +13378,13 @@
         <v>1036</v>
       </c>
       <c r="B476" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="C476" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D476" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="E476" s="5" t="s">
         <v>821</v>
@@ -13398,13 +13398,13 @@
         <v>1036</v>
       </c>
       <c r="B477" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="C477" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D477" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="E477" s="5" t="s">
         <v>821</v>
@@ -13418,13 +13418,13 @@
         <v>1036</v>
       </c>
       <c r="B478" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C478" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D478" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="E478" s="5" t="s">
         <v>821</v>
@@ -13438,13 +13438,13 @@
         <v>1036</v>
       </c>
       <c r="B479" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="C479" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D479" s="3" t="s">
-        <v>1134</v>
+        <v>525</v>
       </c>
       <c r="E479" s="5" t="s">
         <v>821</v>
@@ -13458,13 +13458,13 @@
         <v>1036</v>
       </c>
       <c r="B480" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C480" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D480" s="3" t="s">
-        <v>525</v>
+        <v>1135</v>
       </c>
       <c r="E480" s="5" t="s">
         <v>821</v>
@@ -13478,13 +13478,13 @@
         <v>1036</v>
       </c>
       <c r="B481" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C481" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D481" s="3" t="s">
-        <v>1135</v>
+        <v>522</v>
       </c>
       <c r="E481" s="5" t="s">
         <v>821</v>
@@ -13498,13 +13498,13 @@
         <v>1036</v>
       </c>
       <c r="B482" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C482" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D482" s="3" t="s">
-        <v>522</v>
+        <v>1136</v>
       </c>
       <c r="E482" s="5" t="s">
         <v>821</v>
@@ -13518,13 +13518,13 @@
         <v>1036</v>
       </c>
       <c r="B483" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="C483" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D483" s="3" t="s">
-        <v>1136</v>
+        <v>517</v>
       </c>
       <c r="E483" s="5" t="s">
         <v>821</v>
@@ -13538,13 +13538,13 @@
         <v>1036</v>
       </c>
       <c r="B484" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C484" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D484" s="3" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="E484" s="5" t="s">
         <v>821</v>
@@ -13558,13 +13558,13 @@
         <v>1036</v>
       </c>
       <c r="B485" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="C485" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D485" s="3" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E485" s="5" t="s">
         <v>821</v>
@@ -13578,13 +13578,13 @@
         <v>1036</v>
       </c>
       <c r="B486" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C486" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D486" s="3" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E486" s="5" t="s">
         <v>821</v>
@@ -13598,13 +13598,13 @@
         <v>1036</v>
       </c>
       <c r="B487" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="C487" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D487" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E487" s="5" t="s">
         <v>821</v>
@@ -13618,13 +13618,13 @@
         <v>1036</v>
       </c>
       <c r="B488" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="C488" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D488" s="3" t="s">
-        <v>521</v>
+        <v>841</v>
       </c>
       <c r="E488" s="5" t="s">
         <v>821</v>
@@ -13638,13 +13638,13 @@
         <v>1036</v>
       </c>
       <c r="B489" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="C489" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D489" s="3" t="s">
-        <v>841</v>
+        <v>523</v>
       </c>
       <c r="E489" s="5" t="s">
         <v>821</v>
@@ -13658,13 +13658,13 @@
         <v>1036</v>
       </c>
       <c r="B490" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="C490" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D490" s="3" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="E490" s="5" t="s">
         <v>821</v>
@@ -13678,13 +13678,13 @@
         <v>1036</v>
       </c>
       <c r="B491" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="C491" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D491" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E491" s="5" t="s">
         <v>821</v>
@@ -13698,13 +13698,13 @@
         <v>1036</v>
       </c>
       <c r="B492" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="C492" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D492" s="3" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="E492" s="5" t="s">
         <v>821</v>
@@ -13718,13 +13718,13 @@
         <v>1036</v>
       </c>
       <c r="B493" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="C493" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D493" s="3" t="s">
-        <v>537</v>
+        <v>456</v>
       </c>
       <c r="E493" s="5" t="s">
         <v>821</v>
@@ -13738,93 +13738,93 @@
         <v>1036</v>
       </c>
       <c r="B494" t="s">
-        <v>1123</v>
+        <v>1039</v>
       </c>
       <c r="C494" s="10" t="s">
         <v>1124</v>
       </c>
       <c r="D494" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E494" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="F494" s="5" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="495" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>1036</v>
       </c>
       <c r="B495" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="C495" s="10" t="s">
-        <v>1124</v>
+        <v>1064</v>
       </c>
       <c r="D495" s="3" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="496" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1139</v>
+      </c>
+      <c r="E495" s="5" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F495" s="5" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>1036</v>
       </c>
       <c r="B496" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C496" s="10" t="s">
         <v>1064</v>
       </c>
       <c r="D496" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="E496" s="5" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="F496" s="5" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="497" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>1036</v>
       </c>
       <c r="B497" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="C497" s="10" t="s">
         <v>1064</v>
       </c>
       <c r="D497" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="E497" s="5" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="F497" s="5" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="498" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>1036</v>
       </c>
       <c r="B498" t="s">
-        <v>1042</v>
+        <v>1142</v>
       </c>
       <c r="C498" s="10" t="s">
-        <v>1064</v>
+        <v>1149</v>
       </c>
       <c r="D498" s="3" t="s">
-        <v>1141</v>
+        <v>1153</v>
       </c>
       <c r="E498" s="5" t="s">
-        <v>1152</v>
+        <v>821</v>
       </c>
       <c r="F498" s="5" t="s">
-        <v>757</v>
+        <v>822</v>
       </c>
     </row>
     <row r="499" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -13832,13 +13832,13 @@
         <v>1036</v>
       </c>
       <c r="B499" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C499" s="10" t="s">
         <v>1149</v>
       </c>
       <c r="D499" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="E499" s="5" t="s">
         <v>821</v>
@@ -13852,13 +13852,13 @@
         <v>1036</v>
       </c>
       <c r="B500" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="C500" s="10" t="s">
         <v>1149</v>
       </c>
       <c r="D500" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="E500" s="5" t="s">
         <v>821</v>
@@ -13872,13 +13872,13 @@
         <v>1036</v>
       </c>
       <c r="B501" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="C501" s="10" t="s">
         <v>1149</v>
       </c>
       <c r="D501" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="E501" s="5" t="s">
         <v>821</v>
@@ -13892,13 +13892,13 @@
         <v>1036</v>
       </c>
       <c r="B502" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="C502" s="10" t="s">
         <v>1149</v>
       </c>
       <c r="D502" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="E502" s="5" t="s">
         <v>821</v>
@@ -13912,13 +13912,13 @@
         <v>1036</v>
       </c>
       <c r="B503" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C503" s="10" t="s">
         <v>1149</v>
       </c>
       <c r="D503" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="E503" s="5" t="s">
         <v>821</v>
@@ -13932,13 +13932,13 @@
         <v>1036</v>
       </c>
       <c r="B504" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="C504" s="10" t="s">
         <v>1149</v>
       </c>
       <c r="D504" s="3" t="s">
-        <v>1158</v>
+        <v>456</v>
       </c>
       <c r="E504" s="5" t="s">
         <v>821</v>
@@ -13952,33 +13952,33 @@
         <v>1036</v>
       </c>
       <c r="B505" t="s">
-        <v>1148</v>
+        <v>1043</v>
       </c>
       <c r="C505" s="10" t="s">
         <v>1149</v>
       </c>
       <c r="D505" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E505" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="F505" s="5" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="506" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>1036</v>
       </c>
       <c r="B506" t="s">
-        <v>1043</v>
+        <v>1159</v>
       </c>
       <c r="C506" s="10" t="s">
-        <v>1149</v>
+        <v>1165</v>
       </c>
       <c r="D506" s="3" t="s">
-        <v>1093</v>
+        <v>1166</v>
+      </c>
+      <c r="E506" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="F506" s="5" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="507" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -13986,13 +13986,13 @@
         <v>1036</v>
       </c>
       <c r="B507" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="C507" s="10" t="s">
         <v>1165</v>
       </c>
       <c r="D507" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="E507" s="5" t="s">
         <v>821</v>
@@ -14006,13 +14006,13 @@
         <v>1036</v>
       </c>
       <c r="B508" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="C508" s="10" t="s">
         <v>1165</v>
       </c>
-      <c r="D508" s="3" t="s">
-        <v>1167</v>
+      <c r="D508" s="5" t="s">
+        <v>1168</v>
       </c>
       <c r="E508" s="5" t="s">
         <v>821</v>
@@ -14026,13 +14026,13 @@
         <v>1036</v>
       </c>
       <c r="B509" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="C509" s="10" t="s">
         <v>1165</v>
       </c>
-      <c r="D509" s="5" t="s">
-        <v>1168</v>
+      <c r="D509" s="3" t="s">
+        <v>1169</v>
       </c>
       <c r="E509" s="5" t="s">
         <v>821</v>
@@ -14046,13 +14046,13 @@
         <v>1036</v>
       </c>
       <c r="B510" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="C510" s="10" t="s">
         <v>1165</v>
       </c>
       <c r="D510" s="3" t="s">
-        <v>1169</v>
+        <v>456</v>
       </c>
       <c r="E510" s="5" t="s">
         <v>821</v>
@@ -14066,13 +14066,13 @@
         <v>1036</v>
       </c>
       <c r="B511" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="C511" s="10" t="s">
         <v>1165</v>
       </c>
       <c r="D511" s="3" t="s">
-        <v>456</v>
+        <v>1170</v>
       </c>
       <c r="E511" s="5" t="s">
         <v>821</v>
@@ -14086,19 +14086,13 @@
         <v>1036</v>
       </c>
       <c r="B512" t="s">
-        <v>1164</v>
+        <v>1044</v>
       </c>
       <c r="C512" s="10" t="s">
         <v>1165</v>
       </c>
       <c r="D512" s="3" t="s">
-        <v>1170</v>
-      </c>
-      <c r="E512" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="F512" s="5" t="s">
-        <v>822</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="513" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -14106,13 +14100,19 @@
         <v>1036</v>
       </c>
       <c r="B513" t="s">
-        <v>1044</v>
+        <v>1171</v>
       </c>
       <c r="C513" s="10" t="s">
-        <v>1165</v>
+        <v>1197</v>
       </c>
       <c r="D513" s="3" t="s">
-        <v>1093</v>
+        <v>1126</v>
+      </c>
+      <c r="E513" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="F513" s="5" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="514" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -14120,13 +14120,13 @@
         <v>1036</v>
       </c>
       <c r="B514" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="C514" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D514" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="E514" s="5" t="s">
         <v>821</v>
@@ -14140,13 +14140,13 @@
         <v>1036</v>
       </c>
       <c r="B515" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="C515" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D515" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="E515" s="5" t="s">
         <v>821</v>
@@ -14160,13 +14160,13 @@
         <v>1036</v>
       </c>
       <c r="B516" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="C516" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D516" s="3" t="s">
-        <v>1128</v>
+        <v>527</v>
       </c>
       <c r="E516" s="5" t="s">
         <v>821</v>
@@ -14180,13 +14180,13 @@
         <v>1036</v>
       </c>
       <c r="B517" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="C517" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D517" s="3" t="s">
-        <v>527</v>
+        <v>1129</v>
       </c>
       <c r="E517" s="5" t="s">
         <v>821</v>
@@ -14200,13 +14200,13 @@
         <v>1036</v>
       </c>
       <c r="B518" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="C518" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D518" s="3" t="s">
-        <v>1129</v>
+        <v>519</v>
       </c>
       <c r="E518" s="5" t="s">
         <v>821</v>
@@ -14220,13 +14220,13 @@
         <v>1036</v>
       </c>
       <c r="B519" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="C519" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D519" s="3" t="s">
-        <v>519</v>
+        <v>1130</v>
       </c>
       <c r="E519" s="5" t="s">
         <v>821</v>
@@ -14240,13 +14240,13 @@
         <v>1036</v>
       </c>
       <c r="B520" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="C520" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D520" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="E520" s="5" t="s">
         <v>821</v>
@@ -14260,13 +14260,13 @@
         <v>1036</v>
       </c>
       <c r="B521" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="C521" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D521" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="E521" s="5" t="s">
         <v>821</v>
@@ -14280,13 +14280,13 @@
         <v>1036</v>
       </c>
       <c r="B522" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="C522" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D522" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="E522" s="5" t="s">
         <v>821</v>
@@ -14300,13 +14300,13 @@
         <v>1036</v>
       </c>
       <c r="B523" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="C523" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D523" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="E523" s="5" t="s">
         <v>821</v>
@@ -14320,13 +14320,13 @@
         <v>1036</v>
       </c>
       <c r="B524" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="C524" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D524" s="3" t="s">
-        <v>1134</v>
+        <v>525</v>
       </c>
       <c r="E524" s="5" t="s">
         <v>821</v>
@@ -14340,13 +14340,13 @@
         <v>1036</v>
       </c>
       <c r="B525" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="C525" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D525" s="3" t="s">
-        <v>525</v>
+        <v>1135</v>
       </c>
       <c r="E525" s="5" t="s">
         <v>821</v>
@@ -14360,13 +14360,13 @@
         <v>1036</v>
       </c>
       <c r="B526" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="C526" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D526" s="3" t="s">
-        <v>1135</v>
+        <v>522</v>
       </c>
       <c r="E526" s="5" t="s">
         <v>821</v>
@@ -14380,13 +14380,13 @@
         <v>1036</v>
       </c>
       <c r="B527" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="C527" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D527" s="3" t="s">
-        <v>522</v>
+        <v>1136</v>
       </c>
       <c r="E527" s="5" t="s">
         <v>821</v>
@@ -14400,13 +14400,13 @@
         <v>1036</v>
       </c>
       <c r="B528" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="C528" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D528" s="3" t="s">
-        <v>1136</v>
+        <v>517</v>
       </c>
       <c r="E528" s="5" t="s">
         <v>821</v>
@@ -14420,13 +14420,13 @@
         <v>1036</v>
       </c>
       <c r="B529" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="C529" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D529" s="3" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="E529" s="5" t="s">
         <v>821</v>
@@ -14440,13 +14440,13 @@
         <v>1036</v>
       </c>
       <c r="B530" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="C530" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D530" s="3" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E530" s="5" t="s">
         <v>821</v>
@@ -14460,13 +14460,13 @@
         <v>1036</v>
       </c>
       <c r="B531" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="C531" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D531" s="3" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E531" s="5" t="s">
         <v>821</v>
@@ -14480,13 +14480,13 @@
         <v>1036</v>
       </c>
       <c r="B532" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="C532" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D532" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E532" s="5" t="s">
         <v>821</v>
@@ -14500,13 +14500,13 @@
         <v>1036</v>
       </c>
       <c r="B533" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="C533" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D533" s="3" t="s">
-        <v>521</v>
+        <v>841</v>
       </c>
       <c r="E533" s="5" t="s">
         <v>821</v>
@@ -14520,13 +14520,13 @@
         <v>1036</v>
       </c>
       <c r="B534" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="C534" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D534" s="3" t="s">
-        <v>841</v>
+        <v>523</v>
       </c>
       <c r="E534" s="5" t="s">
         <v>821</v>
@@ -14540,13 +14540,13 @@
         <v>1036</v>
       </c>
       <c r="B535" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="C535" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D535" s="3" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="E535" s="5" t="s">
         <v>821</v>
@@ -14560,13 +14560,13 @@
         <v>1036</v>
       </c>
       <c r="B536" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="C536" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D536" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E536" s="5" t="s">
         <v>821</v>
@@ -14580,13 +14580,13 @@
         <v>1036</v>
       </c>
       <c r="B537" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="C537" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D537" s="3" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="E537" s="5" t="s">
         <v>821</v>
@@ -14600,13 +14600,13 @@
         <v>1036</v>
       </c>
       <c r="B538" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="C538" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D538" s="3" t="s">
-        <v>537</v>
+        <v>456</v>
       </c>
       <c r="E538" s="5" t="s">
         <v>821</v>
@@ -14620,33 +14620,33 @@
         <v>1036</v>
       </c>
       <c r="B539" t="s">
-        <v>1196</v>
+        <v>1045</v>
       </c>
       <c r="C539" s="10" t="s">
         <v>1197</v>
       </c>
       <c r="D539" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E539" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="F539" s="5" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="540" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>1036</v>
       </c>
       <c r="B540" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="C540" s="10" t="s">
-        <v>1197</v>
+        <v>1065</v>
       </c>
       <c r="D540" s="3" t="s">
-        <v>1093</v>
+        <v>1198</v>
+      </c>
+      <c r="E540" s="5" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F540" s="5" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="541" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -14654,19 +14654,19 @@
         <v>1036</v>
       </c>
       <c r="B541" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C541" s="10" t="s">
         <v>1065</v>
       </c>
       <c r="D541" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="E541" s="5" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="F541" s="5" t="s">
-        <v>757</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="542" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -14674,19 +14674,13 @@
         <v>1036</v>
       </c>
       <c r="B542" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="C542" s="10" t="s">
         <v>1065</v>
       </c>
       <c r="D542" s="3" t="s">
-        <v>1199</v>
-      </c>
-      <c r="E542" s="5" t="s">
-        <v>1206</v>
-      </c>
-      <c r="F542" s="5" t="s">
-        <v>1207</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="543" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -14694,13 +14688,19 @@
         <v>1036</v>
       </c>
       <c r="B543" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="C543" s="10" t="s">
         <v>1065</v>
       </c>
       <c r="D543" s="3" t="s">
-        <v>1200</v>
+        <v>1201</v>
+      </c>
+      <c r="E543" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="F543" s="5" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="544" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -14708,13 +14708,13 @@
         <v>1036</v>
       </c>
       <c r="B544" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C544" s="10" t="s">
         <v>1065</v>
       </c>
       <c r="D544" s="3" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="E544" s="5" t="s">
         <v>799</v>
@@ -14728,13 +14728,13 @@
         <v>1036</v>
       </c>
       <c r="B545" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C545" s="10" t="s">
         <v>1065</v>
       </c>
       <c r="D545" s="3" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="E545" s="5" t="s">
         <v>799</v>
@@ -14748,13 +14748,13 @@
         <v>1036</v>
       </c>
       <c r="B546" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C546" s="10" t="s">
         <v>1065</v>
       </c>
       <c r="D546" s="3" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="E546" s="5" t="s">
         <v>799</v>
@@ -14763,24 +14763,24 @@
         <v>773</v>
       </c>
     </row>
-    <row r="547" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>1036</v>
       </c>
       <c r="B547" t="s">
-        <v>1052</v>
+        <v>1209</v>
       </c>
       <c r="C547" s="10" t="s">
-        <v>1065</v>
+        <v>1208</v>
       </c>
       <c r="D547" s="3" t="s">
-        <v>1204</v>
+        <v>1126</v>
       </c>
       <c r="E547" s="5" t="s">
-        <v>799</v>
+        <v>821</v>
       </c>
       <c r="F547" s="5" t="s">
-        <v>773</v>
+        <v>822</v>
       </c>
     </row>
     <row r="548" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -14788,13 +14788,13 @@
         <v>1036</v>
       </c>
       <c r="B548" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="C548" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D548" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="E548" s="5" t="s">
         <v>821</v>
@@ -14808,13 +14808,13 @@
         <v>1036</v>
       </c>
       <c r="B549" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="C549" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D549" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="E549" s="5" t="s">
         <v>821</v>
@@ -14828,13 +14828,13 @@
         <v>1036</v>
       </c>
       <c r="B550" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="C550" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D550" s="3" t="s">
-        <v>1128</v>
+        <v>527</v>
       </c>
       <c r="E550" s="5" t="s">
         <v>821</v>
@@ -14848,13 +14848,13 @@
         <v>1036</v>
       </c>
       <c r="B551" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="C551" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D551" s="3" t="s">
-        <v>527</v>
+        <v>1129</v>
       </c>
       <c r="E551" s="5" t="s">
         <v>821</v>
@@ -14868,13 +14868,13 @@
         <v>1036</v>
       </c>
       <c r="B552" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="C552" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D552" s="3" t="s">
-        <v>1129</v>
+        <v>519</v>
       </c>
       <c r="E552" s="5" t="s">
         <v>821</v>
@@ -14888,13 +14888,13 @@
         <v>1036</v>
       </c>
       <c r="B553" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="C553" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D553" s="3" t="s">
-        <v>519</v>
+        <v>1130</v>
       </c>
       <c r="E553" s="5" t="s">
         <v>821</v>
@@ -14908,13 +14908,13 @@
         <v>1036</v>
       </c>
       <c r="B554" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="C554" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D554" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="E554" s="5" t="s">
         <v>821</v>
@@ -14928,13 +14928,13 @@
         <v>1036</v>
       </c>
       <c r="B555" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="C555" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D555" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="E555" s="5" t="s">
         <v>821</v>
@@ -14948,13 +14948,13 @@
         <v>1036</v>
       </c>
       <c r="B556" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="C556" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D556" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="E556" s="5" t="s">
         <v>821</v>
@@ -14968,13 +14968,13 @@
         <v>1036</v>
       </c>
       <c r="B557" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="C557" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D557" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="E557" s="5" t="s">
         <v>821</v>
@@ -14988,13 +14988,13 @@
         <v>1036</v>
       </c>
       <c r="B558" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="C558" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D558" s="3" t="s">
-        <v>1134</v>
+        <v>525</v>
       </c>
       <c r="E558" s="5" t="s">
         <v>821</v>
@@ -15008,13 +15008,13 @@
         <v>1036</v>
       </c>
       <c r="B559" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="C559" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D559" s="3" t="s">
-        <v>525</v>
+        <v>1135</v>
       </c>
       <c r="E559" s="5" t="s">
         <v>821</v>
@@ -15028,13 +15028,13 @@
         <v>1036</v>
       </c>
       <c r="B560" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="C560" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D560" s="3" t="s">
-        <v>1135</v>
+        <v>522</v>
       </c>
       <c r="E560" s="5" t="s">
         <v>821</v>
@@ -15048,13 +15048,13 @@
         <v>1036</v>
       </c>
       <c r="B561" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="C561" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D561" s="3" t="s">
-        <v>522</v>
+        <v>1136</v>
       </c>
       <c r="E561" s="5" t="s">
         <v>821</v>
@@ -15068,13 +15068,13 @@
         <v>1036</v>
       </c>
       <c r="B562" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="C562" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D562" s="3" t="s">
-        <v>1136</v>
+        <v>517</v>
       </c>
       <c r="E562" s="5" t="s">
         <v>821</v>
@@ -15088,13 +15088,13 @@
         <v>1036</v>
       </c>
       <c r="B563" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C563" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D563" s="3" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="E563" s="5" t="s">
         <v>821</v>
@@ -15108,13 +15108,13 @@
         <v>1036</v>
       </c>
       <c r="B564" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="C564" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D564" s="3" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E564" s="5" t="s">
         <v>821</v>
@@ -15128,13 +15128,13 @@
         <v>1036</v>
       </c>
       <c r="B565" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="C565" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D565" s="3" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E565" s="5" t="s">
         <v>821</v>
@@ -15148,13 +15148,13 @@
         <v>1036</v>
       </c>
       <c r="B566" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="C566" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D566" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E566" s="5" t="s">
         <v>821</v>
@@ -15168,13 +15168,13 @@
         <v>1036</v>
       </c>
       <c r="B567" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="C567" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D567" s="3" t="s">
-        <v>521</v>
+        <v>841</v>
       </c>
       <c r="E567" s="5" t="s">
         <v>821</v>
@@ -15188,13 +15188,13 @@
         <v>1036</v>
       </c>
       <c r="B568" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="C568" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D568" s="3" t="s">
-        <v>841</v>
+        <v>523</v>
       </c>
       <c r="E568" s="5" t="s">
         <v>821</v>
@@ -15208,13 +15208,13 @@
         <v>1036</v>
       </c>
       <c r="B569" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="C569" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D569" s="3" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="E569" s="5" t="s">
         <v>821</v>
@@ -15228,13 +15228,13 @@
         <v>1036</v>
       </c>
       <c r="B570" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="C570" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D570" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E570" s="5" t="s">
         <v>821</v>
@@ -15248,13 +15248,13 @@
         <v>1036</v>
       </c>
       <c r="B571" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="C571" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D571" s="3" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="E571" s="5" t="s">
         <v>821</v>
@@ -15268,13 +15268,13 @@
         <v>1036</v>
       </c>
       <c r="B572" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="C572" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D572" s="3" t="s">
-        <v>537</v>
+        <v>456</v>
       </c>
       <c r="E572" s="5" t="s">
         <v>821</v>
@@ -15288,33 +15288,33 @@
         <v>1036</v>
       </c>
       <c r="B573" t="s">
-        <v>1234</v>
+        <v>1053</v>
       </c>
       <c r="C573" s="10" t="s">
         <v>1208</v>
       </c>
       <c r="D573" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E573" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="F573" s="5" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="574" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="574" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
         <v>1036</v>
       </c>
       <c r="B574" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="C574" s="10" t="s">
-        <v>1208</v>
+        <v>1066</v>
       </c>
       <c r="D574" s="3" t="s">
-        <v>1093</v>
+        <v>1235</v>
+      </c>
+      <c r="E574" s="5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F574" s="5" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="575" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -15322,19 +15322,13 @@
         <v>1036</v>
       </c>
       <c r="B575" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="C575" s="10" t="s">
         <v>1066</v>
       </c>
       <c r="D575" s="3" t="s">
-        <v>1235</v>
-      </c>
-      <c r="E575" s="5" t="s">
-        <v>1236</v>
-      </c>
-      <c r="F575" s="5" t="s">
-        <v>759</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="576" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -15342,47 +15336,47 @@
         <v>1036</v>
       </c>
       <c r="B576" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="C576" s="10" t="s">
         <v>1066</v>
       </c>
       <c r="D576" s="3" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="577" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1238</v>
+      </c>
+      <c r="E576" s="5" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F576" s="5" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="577" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>1036</v>
       </c>
       <c r="B577" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C577" s="10" t="s">
         <v>1066</v>
       </c>
       <c r="D577" s="3" t="s">
-        <v>1238</v>
-      </c>
-      <c r="E577" s="5" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F577" s="5" t="s">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="578" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="578" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>1036</v>
       </c>
       <c r="B578" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="C578" s="10" t="s">
         <v>1066</v>
       </c>
       <c r="D578" s="3" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="579" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -15390,53 +15384,53 @@
         <v>1036</v>
       </c>
       <c r="B579" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="C579" s="10" t="s">
         <v>1066</v>
       </c>
       <c r="D579" s="3" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="580" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1243</v>
+      </c>
+      <c r="E579" s="5" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F579" s="5" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="580" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>1036</v>
       </c>
       <c r="B580" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C580" s="10" t="s">
         <v>1066</v>
       </c>
       <c r="D580" s="3" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="E580" s="5" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
       <c r="F580" s="5" t="s">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="581" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="581" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>1036</v>
       </c>
       <c r="B581" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C581" s="10" t="s">
         <v>1066</v>
       </c>
       <c r="D581" s="3" t="s">
-        <v>1245</v>
-      </c>
-      <c r="E581" s="5" t="s">
-        <v>1246</v>
-      </c>
-      <c r="F581" s="5" t="s">
-        <v>759</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="582" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -15444,35 +15438,41 @@
         <v>1036</v>
       </c>
       <c r="B582" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="C582" s="10" t="s">
         <v>1066</v>
       </c>
       <c r="D582" s="3" t="s">
-        <v>1247</v>
-      </c>
-    </row>
-    <row r="583" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>1036</v>
       </c>
       <c r="B583" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="C583" s="10" t="s">
-        <v>1066</v>
+        <v>389</v>
       </c>
       <c r="D583" s="3" t="s">
-        <v>1248</v>
+        <v>423</v>
+      </c>
+      <c r="E583" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="F583" s="5" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="584" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
-        <v>1036</v>
+        <v>385</v>
       </c>
       <c r="B584" t="s">
-        <v>1063</v>
+        <v>350</v>
       </c>
       <c r="C584" s="10" t="s">
         <v>389</v>

</xml_diff>